<commit_message>
added files and OOP
</commit_message>
<xml_diff>
--- a/Finance-TP1-RAROC.xlsx
+++ b/Finance-TP1-RAROC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentin/Desktop/TSP/3A/Risques financiers/tp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CA3F87-5871-5B4C-9A39-8A002162F74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00B118A-1276-214E-9E93-335482BC042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="26660" windowHeight="16900" xr2:uid="{06508FD0-9F33-7140-9185-849472C81A33}"/>
   </bookViews>
@@ -2549,7 +2549,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="25">
         <f ca="1">TODAY()</f>
-        <v>44481</v>
+        <v>44491</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -2577,7 +2577,7 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="25">
         <f ca="1">DATE(YEAR(B7),MONTH(B7)+1,DAY(B7))</f>
-        <v>44512</v>
+        <v>44522</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -2610,7 +2610,7 @@
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="25">
         <f ca="1">DATE(YEAR(B8),MONTH(B8)+1,DAY(B8))</f>
-        <v>44542</v>
+        <v>44552</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
@@ -2643,7 +2643,7 @@
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="25">
         <f t="shared" ref="B10:B73" ca="1" si="6">DATE(YEAR(B9),MONTH(B9)+1,DAY(B9))</f>
-        <v>44573</v>
+        <v>44583</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -2676,7 +2676,7 @@
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44604</v>
+        <v>44614</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
@@ -2709,7 +2709,7 @@
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44632</v>
+        <v>44642</v>
       </c>
       <c r="C12" s="5">
         <v>5</v>
@@ -2742,7 +2742,7 @@
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44663</v>
+        <v>44673</v>
       </c>
       <c r="C13" s="5">
         <v>6</v>
@@ -2775,7 +2775,7 @@
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44693</v>
+        <v>44703</v>
       </c>
       <c r="C14" s="5">
         <v>7</v>
@@ -2808,7 +2808,7 @@
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44724</v>
+        <v>44734</v>
       </c>
       <c r="C15" s="5">
         <v>8</v>
@@ -2841,7 +2841,7 @@
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44754</v>
+        <v>44764</v>
       </c>
       <c r="C16" s="5">
         <v>9</v>
@@ -2874,7 +2874,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44785</v>
+        <v>44795</v>
       </c>
       <c r="C17" s="5">
         <v>10</v>
@@ -2907,7 +2907,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44816</v>
+        <v>44826</v>
       </c>
       <c r="C18" s="5">
         <v>11</v>
@@ -2940,7 +2940,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44846</v>
+        <v>44856</v>
       </c>
       <c r="C19" s="5">
         <v>12</v>
@@ -2973,7 +2973,7 @@
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44877</v>
+        <v>44887</v>
       </c>
       <c r="C20" s="5">
         <v>13</v>
@@ -3006,7 +3006,7 @@
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44907</v>
+        <v>44917</v>
       </c>
       <c r="C21" s="5">
         <v>14</v>
@@ -3039,7 +3039,7 @@
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44938</v>
+        <v>44948</v>
       </c>
       <c r="C22" s="5">
         <v>15</v>
@@ -3072,7 +3072,7 @@
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44969</v>
+        <v>44979</v>
       </c>
       <c r="C23" s="5">
         <v>16</v>
@@ -3105,7 +3105,7 @@
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44997</v>
+        <v>45007</v>
       </c>
       <c r="C24" s="5">
         <v>17</v>
@@ -3138,7 +3138,7 @@
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45028</v>
+        <v>45038</v>
       </c>
       <c r="C25" s="5">
         <v>18</v>
@@ -3171,7 +3171,7 @@
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45058</v>
+        <v>45068</v>
       </c>
       <c r="C26" s="5">
         <v>19</v>
@@ -3204,7 +3204,7 @@
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45089</v>
+        <v>45099</v>
       </c>
       <c r="C27" s="5">
         <v>20</v>
@@ -3237,7 +3237,7 @@
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45119</v>
+        <v>45129</v>
       </c>
       <c r="C28" s="5">
         <v>21</v>
@@ -3270,7 +3270,7 @@
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45150</v>
+        <v>45160</v>
       </c>
       <c r="C29" s="5">
         <v>22</v>
@@ -3303,7 +3303,7 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45181</v>
+        <v>45191</v>
       </c>
       <c r="C30" s="5">
         <v>23</v>
@@ -3336,7 +3336,7 @@
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45211</v>
+        <v>45221</v>
       </c>
       <c r="C31" s="5">
         <v>24</v>
@@ -3369,7 +3369,7 @@
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45242</v>
+        <v>45252</v>
       </c>
       <c r="C32" s="5">
         <v>25</v>
@@ -3402,7 +3402,7 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45272</v>
+        <v>45282</v>
       </c>
       <c r="C33" s="5">
         <v>26</v>
@@ -3435,7 +3435,7 @@
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45303</v>
+        <v>45313</v>
       </c>
       <c r="C34" s="5">
         <v>27</v>
@@ -3468,7 +3468,7 @@
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45334</v>
+        <v>45344</v>
       </c>
       <c r="C35" s="5">
         <v>28</v>
@@ -3501,7 +3501,7 @@
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45363</v>
+        <v>45373</v>
       </c>
       <c r="C36" s="5">
         <v>29</v>
@@ -3534,7 +3534,7 @@
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45394</v>
+        <v>45404</v>
       </c>
       <c r="C37" s="5">
         <v>30</v>
@@ -3567,7 +3567,7 @@
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45424</v>
+        <v>45434</v>
       </c>
       <c r="C38" s="5">
         <v>31</v>
@@ -3600,7 +3600,7 @@
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45455</v>
+        <v>45465</v>
       </c>
       <c r="C39" s="5">
         <v>32</v>
@@ -3633,7 +3633,7 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45485</v>
+        <v>45495</v>
       </c>
       <c r="C40" s="5">
         <v>33</v>
@@ -3666,7 +3666,7 @@
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45516</v>
+        <v>45526</v>
       </c>
       <c r="C41" s="5">
         <v>34</v>
@@ -3699,7 +3699,7 @@
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45547</v>
+        <v>45557</v>
       </c>
       <c r="C42" s="5">
         <v>35</v>
@@ -3732,7 +3732,7 @@
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45577</v>
+        <v>45587</v>
       </c>
       <c r="C43" s="5">
         <v>36</v>
@@ -3765,7 +3765,7 @@
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45608</v>
+        <v>45618</v>
       </c>
       <c r="C44" s="5">
         <v>37</v>
@@ -3798,7 +3798,7 @@
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45638</v>
+        <v>45648</v>
       </c>
       <c r="C45" s="5">
         <v>38</v>
@@ -3831,7 +3831,7 @@
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45669</v>
+        <v>45679</v>
       </c>
       <c r="C46" s="5">
         <v>39</v>
@@ -3864,7 +3864,7 @@
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45700</v>
+        <v>45710</v>
       </c>
       <c r="C47" s="5">
         <v>40</v>
@@ -3897,7 +3897,7 @@
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45728</v>
+        <v>45738</v>
       </c>
       <c r="C48" s="5">
         <v>41</v>
@@ -3930,7 +3930,7 @@
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45759</v>
+        <v>45769</v>
       </c>
       <c r="C49" s="5">
         <v>42</v>
@@ -3963,7 +3963,7 @@
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45789</v>
+        <v>45799</v>
       </c>
       <c r="C50" s="5">
         <v>43</v>
@@ -3996,7 +3996,7 @@
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45820</v>
+        <v>45830</v>
       </c>
       <c r="C51" s="5">
         <v>44</v>
@@ -4029,7 +4029,7 @@
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45850</v>
+        <v>45860</v>
       </c>
       <c r="C52" s="5">
         <v>45</v>
@@ -4062,7 +4062,7 @@
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45881</v>
+        <v>45891</v>
       </c>
       <c r="C53" s="5">
         <v>46</v>
@@ -4095,7 +4095,7 @@
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45912</v>
+        <v>45922</v>
       </c>
       <c r="C54" s="5">
         <v>47</v>
@@ -4128,7 +4128,7 @@
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45942</v>
+        <v>45952</v>
       </c>
       <c r="C55" s="5">
         <v>48</v>
@@ -4161,7 +4161,7 @@
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45973</v>
+        <v>45983</v>
       </c>
       <c r="C56" s="5">
         <v>49</v>
@@ -4194,7 +4194,7 @@
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46003</v>
+        <v>46013</v>
       </c>
       <c r="C57" s="5">
         <v>50</v>
@@ -4227,7 +4227,7 @@
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46034</v>
+        <v>46044</v>
       </c>
       <c r="C58" s="5">
         <v>51</v>
@@ -4260,7 +4260,7 @@
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46065</v>
+        <v>46075</v>
       </c>
       <c r="C59" s="5">
         <v>52</v>
@@ -4293,7 +4293,7 @@
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46093</v>
+        <v>46103</v>
       </c>
       <c r="C60" s="5">
         <v>53</v>
@@ -4326,7 +4326,7 @@
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46124</v>
+        <v>46134</v>
       </c>
       <c r="C61" s="5">
         <v>54</v>
@@ -4359,7 +4359,7 @@
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46154</v>
+        <v>46164</v>
       </c>
       <c r="C62" s="5">
         <v>55</v>
@@ -4392,7 +4392,7 @@
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46185</v>
+        <v>46195</v>
       </c>
       <c r="C63" s="5">
         <v>56</v>
@@ -4425,7 +4425,7 @@
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46215</v>
+        <v>46225</v>
       </c>
       <c r="C64" s="5">
         <v>57</v>
@@ -4458,7 +4458,7 @@
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46246</v>
+        <v>46256</v>
       </c>
       <c r="C65" s="5">
         <v>58</v>
@@ -4491,7 +4491,7 @@
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46277</v>
+        <v>46287</v>
       </c>
       <c r="C66" s="5">
         <v>59</v>
@@ -4524,7 +4524,7 @@
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46307</v>
+        <v>46317</v>
       </c>
       <c r="C67" s="5">
         <v>60</v>
@@ -4557,7 +4557,7 @@
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46338</v>
+        <v>46348</v>
       </c>
       <c r="C68" s="5">
         <v>61</v>
@@ -4590,7 +4590,7 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46368</v>
+        <v>46378</v>
       </c>
       <c r="C69" s="5">
         <v>62</v>
@@ -4623,7 +4623,7 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46399</v>
+        <v>46409</v>
       </c>
       <c r="C70" s="5">
         <v>63</v>
@@ -4656,7 +4656,7 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46430</v>
+        <v>46440</v>
       </c>
       <c r="C71" s="5">
         <v>64</v>
@@ -4689,7 +4689,7 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46458</v>
+        <v>46468</v>
       </c>
       <c r="C72" s="5">
         <v>65</v>
@@ -4722,7 +4722,7 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46489</v>
+        <v>46499</v>
       </c>
       <c r="C73" s="5">
         <v>66</v>
@@ -4755,7 +4755,7 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="25">
         <f t="shared" ref="B74:B137" ca="1" si="14">DATE(YEAR(B73),MONTH(B73)+1,DAY(B73))</f>
-        <v>46519</v>
+        <v>46529</v>
       </c>
       <c r="C74" s="5">
         <v>67</v>
@@ -4788,7 +4788,7 @@
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46550</v>
+        <v>46560</v>
       </c>
       <c r="C75" s="5">
         <v>68</v>
@@ -4821,7 +4821,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46580</v>
+        <v>46590</v>
       </c>
       <c r="C76" s="5">
         <v>69</v>
@@ -4854,7 +4854,7 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46611</v>
+        <v>46621</v>
       </c>
       <c r="C77" s="5">
         <v>70</v>
@@ -4887,7 +4887,7 @@
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46642</v>
+        <v>46652</v>
       </c>
       <c r="C78" s="5">
         <v>71</v>
@@ -4920,7 +4920,7 @@
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46672</v>
+        <v>46682</v>
       </c>
       <c r="C79" s="5">
         <v>72</v>
@@ -4953,7 +4953,7 @@
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46703</v>
+        <v>46713</v>
       </c>
       <c r="C80" s="5">
         <v>73</v>
@@ -4986,7 +4986,7 @@
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46733</v>
+        <v>46743</v>
       </c>
       <c r="C81" s="5">
         <v>74</v>
@@ -5019,7 +5019,7 @@
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46764</v>
+        <v>46774</v>
       </c>
       <c r="C82" s="5">
         <v>75</v>
@@ -5052,7 +5052,7 @@
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46795</v>
+        <v>46805</v>
       </c>
       <c r="C83" s="5">
         <v>76</v>
@@ -5085,7 +5085,7 @@
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46824</v>
+        <v>46834</v>
       </c>
       <c r="C84" s="5">
         <v>77</v>
@@ -5118,7 +5118,7 @@
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46855</v>
+        <v>46865</v>
       </c>
       <c r="C85" s="5">
         <v>78</v>
@@ -5151,7 +5151,7 @@
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46885</v>
+        <v>46895</v>
       </c>
       <c r="C86" s="5">
         <v>79</v>
@@ -5184,7 +5184,7 @@
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46916</v>
+        <v>46926</v>
       </c>
       <c r="C87" s="5">
         <v>80</v>
@@ -5217,7 +5217,7 @@
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46946</v>
+        <v>46956</v>
       </c>
       <c r="C88" s="5">
         <v>81</v>
@@ -5250,7 +5250,7 @@
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46977</v>
+        <v>46987</v>
       </c>
       <c r="C89" s="5">
         <v>82</v>
@@ -5283,7 +5283,7 @@
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47008</v>
+        <v>47018</v>
       </c>
       <c r="C90" s="5">
         <v>83</v>
@@ -5316,7 +5316,7 @@
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47038</v>
+        <v>47048</v>
       </c>
       <c r="C91" s="5">
         <v>84</v>
@@ -5349,7 +5349,7 @@
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47069</v>
+        <v>47079</v>
       </c>
       <c r="C92" s="5">
         <v>85</v>
@@ -5382,7 +5382,7 @@
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47099</v>
+        <v>47109</v>
       </c>
       <c r="C93" s="5">
         <v>86</v>
@@ -5415,7 +5415,7 @@
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47130</v>
+        <v>47140</v>
       </c>
       <c r="C94" s="5">
         <v>87</v>
@@ -5448,7 +5448,7 @@
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47161</v>
+        <v>47171</v>
       </c>
       <c r="C95" s="5">
         <v>88</v>
@@ -5481,7 +5481,7 @@
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47189</v>
+        <v>47199</v>
       </c>
       <c r="C96" s="5">
         <v>89</v>
@@ -5514,7 +5514,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47220</v>
+        <v>47230</v>
       </c>
       <c r="C97" s="5">
         <v>90</v>
@@ -5547,7 +5547,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47250</v>
+        <v>47260</v>
       </c>
       <c r="C98" s="5">
         <v>91</v>
@@ -5580,7 +5580,7 @@
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47281</v>
+        <v>47291</v>
       </c>
       <c r="C99" s="5">
         <v>92</v>
@@ -5613,7 +5613,7 @@
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47311</v>
+        <v>47321</v>
       </c>
       <c r="C100" s="5">
         <v>93</v>
@@ -5646,7 +5646,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47342</v>
+        <v>47352</v>
       </c>
       <c r="C101" s="5">
         <v>94</v>
@@ -5679,7 +5679,7 @@
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47373</v>
+        <v>47383</v>
       </c>
       <c r="C102" s="5">
         <v>95</v>
@@ -5712,7 +5712,7 @@
     <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47403</v>
+        <v>47413</v>
       </c>
       <c r="C103" s="5">
         <v>96</v>
@@ -5745,7 +5745,7 @@
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47434</v>
+        <v>47444</v>
       </c>
       <c r="C104" s="5">
         <v>97</v>
@@ -5778,7 +5778,7 @@
     <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47464</v>
+        <v>47474</v>
       </c>
       <c r="C105" s="5">
         <v>98</v>
@@ -5811,7 +5811,7 @@
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47495</v>
+        <v>47505</v>
       </c>
       <c r="C106" s="5">
         <v>99</v>
@@ -5844,7 +5844,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47526</v>
+        <v>47536</v>
       </c>
       <c r="C107" s="5">
         <v>100</v>
@@ -5877,7 +5877,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47554</v>
+        <v>47564</v>
       </c>
       <c r="C108" s="5">
         <v>101</v>
@@ -5910,7 +5910,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47585</v>
+        <v>47595</v>
       </c>
       <c r="C109" s="5">
         <v>102</v>
@@ -5943,7 +5943,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47615</v>
+        <v>47625</v>
       </c>
       <c r="C110" s="5">
         <v>103</v>
@@ -5976,7 +5976,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47646</v>
+        <v>47656</v>
       </c>
       <c r="C111" s="5">
         <v>104</v>
@@ -6009,7 +6009,7 @@
     <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47676</v>
+        <v>47686</v>
       </c>
       <c r="C112" s="5">
         <v>105</v>
@@ -6042,7 +6042,7 @@
     <row r="113" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B113" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47707</v>
+        <v>47717</v>
       </c>
       <c r="C113" s="5">
         <v>106</v>
@@ -6075,7 +6075,7 @@
     <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47738</v>
+        <v>47748</v>
       </c>
       <c r="C114" s="5">
         <v>107</v>
@@ -6108,7 +6108,7 @@
     <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B115" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47768</v>
+        <v>47778</v>
       </c>
       <c r="C115" s="5">
         <v>108</v>
@@ -6141,7 +6141,7 @@
     <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B116" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47799</v>
+        <v>47809</v>
       </c>
       <c r="C116" s="5">
         <v>109</v>
@@ -6174,7 +6174,7 @@
     <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47829</v>
+        <v>47839</v>
       </c>
       <c r="C117" s="5">
         <v>110</v>
@@ -6207,7 +6207,7 @@
     <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B118" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47860</v>
+        <v>47870</v>
       </c>
       <c r="C118" s="5">
         <v>111</v>
@@ -6240,7 +6240,7 @@
     <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47891</v>
+        <v>47901</v>
       </c>
       <c r="C119" s="5">
         <v>112</v>
@@ -6273,7 +6273,7 @@
     <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47919</v>
+        <v>47929</v>
       </c>
       <c r="C120" s="5">
         <v>113</v>
@@ -6306,7 +6306,7 @@
     <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47950</v>
+        <v>47960</v>
       </c>
       <c r="C121" s="5">
         <v>114</v>
@@ -6339,7 +6339,7 @@
     <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47980</v>
+        <v>47990</v>
       </c>
       <c r="C122" s="5">
         <v>115</v>
@@ -6372,7 +6372,7 @@
     <row r="123" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B123" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48011</v>
+        <v>48021</v>
       </c>
       <c r="C123" s="5">
         <v>116</v>
@@ -6405,7 +6405,7 @@
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48041</v>
+        <v>48051</v>
       </c>
       <c r="C124" s="5">
         <v>117</v>
@@ -6438,7 +6438,7 @@
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48072</v>
+        <v>48082</v>
       </c>
       <c r="C125" s="5">
         <v>118</v>
@@ -6471,7 +6471,7 @@
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48103</v>
+        <v>48113</v>
       </c>
       <c r="C126" s="5">
         <v>119</v>
@@ -6504,7 +6504,7 @@
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48133</v>
+        <v>48143</v>
       </c>
       <c r="C127" s="5">
         <v>120</v>
@@ -6537,7 +6537,7 @@
     <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48164</v>
+        <v>48174</v>
       </c>
       <c r="C128" s="5">
         <v>121</v>
@@ -6570,7 +6570,7 @@
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48194</v>
+        <v>48204</v>
       </c>
       <c r="C129" s="5">
         <v>122</v>
@@ -6603,7 +6603,7 @@
     <row r="130" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B130" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48225</v>
+        <v>48235</v>
       </c>
       <c r="C130" s="5">
         <v>123</v>
@@ -6636,7 +6636,7 @@
     <row r="131" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B131" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48256</v>
+        <v>48266</v>
       </c>
       <c r="C131" s="5">
         <v>124</v>
@@ -6669,7 +6669,7 @@
     <row r="132" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B132" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48285</v>
+        <v>48295</v>
       </c>
       <c r="C132" s="5">
         <v>125</v>
@@ -6702,7 +6702,7 @@
     <row r="133" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B133" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48316</v>
+        <v>48326</v>
       </c>
       <c r="C133" s="5">
         <v>126</v>
@@ -6735,7 +6735,7 @@
     <row r="134" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B134" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48346</v>
+        <v>48356</v>
       </c>
       <c r="C134" s="5">
         <v>127</v>
@@ -6768,7 +6768,7 @@
     <row r="135" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B135" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48377</v>
+        <v>48387</v>
       </c>
       <c r="C135" s="5">
         <v>128</v>
@@ -6801,7 +6801,7 @@
     <row r="136" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B136" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48407</v>
+        <v>48417</v>
       </c>
       <c r="C136" s="5">
         <v>129</v>
@@ -6834,7 +6834,7 @@
     <row r="137" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B137" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48438</v>
+        <v>48448</v>
       </c>
       <c r="C137" s="5">
         <v>130</v>
@@ -6867,7 +6867,7 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B138" s="25">
         <f t="shared" ref="B138:B201" ca="1" si="21">DATE(YEAR(B137),MONTH(B137)+1,DAY(B137))</f>
-        <v>48469</v>
+        <v>48479</v>
       </c>
       <c r="C138" s="5">
         <v>131</v>
@@ -6900,7 +6900,7 @@
     <row r="139" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B139" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48499</v>
+        <v>48509</v>
       </c>
       <c r="C139" s="5">
         <v>132</v>
@@ -6933,7 +6933,7 @@
     <row r="140" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B140" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48530</v>
+        <v>48540</v>
       </c>
       <c r="C140" s="5">
         <v>133</v>
@@ -6966,7 +6966,7 @@
     <row r="141" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B141" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48560</v>
+        <v>48570</v>
       </c>
       <c r="C141" s="5">
         <v>134</v>
@@ -6999,7 +6999,7 @@
     <row r="142" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B142" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48591</v>
+        <v>48601</v>
       </c>
       <c r="C142" s="5">
         <v>135</v>
@@ -7032,7 +7032,7 @@
     <row r="143" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B143" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48622</v>
+        <v>48632</v>
       </c>
       <c r="C143" s="5">
         <v>136</v>
@@ -7065,7 +7065,7 @@
     <row r="144" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B144" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48650</v>
+        <v>48660</v>
       </c>
       <c r="C144" s="5">
         <v>137</v>
@@ -7098,7 +7098,7 @@
     <row r="145" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B145" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48681</v>
+        <v>48691</v>
       </c>
       <c r="C145" s="5">
         <v>138</v>
@@ -7131,7 +7131,7 @@
     <row r="146" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B146" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48711</v>
+        <v>48721</v>
       </c>
       <c r="C146" s="5">
         <v>139</v>
@@ -7164,7 +7164,7 @@
     <row r="147" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B147" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48742</v>
+        <v>48752</v>
       </c>
       <c r="C147" s="5">
         <v>140</v>
@@ -7197,7 +7197,7 @@
     <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48772</v>
+        <v>48782</v>
       </c>
       <c r="C148" s="5">
         <v>141</v>
@@ -7230,7 +7230,7 @@
     <row r="149" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B149" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48803</v>
+        <v>48813</v>
       </c>
       <c r="C149" s="5">
         <v>142</v>
@@ -7263,7 +7263,7 @@
     <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48834</v>
+        <v>48844</v>
       </c>
       <c r="C150" s="5">
         <v>143</v>
@@ -7296,7 +7296,7 @@
     <row r="151" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B151" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48864</v>
+        <v>48874</v>
       </c>
       <c r="C151" s="5">
         <v>144</v>
@@ -7329,7 +7329,7 @@
     <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48895</v>
+        <v>48905</v>
       </c>
       <c r="C152" s="5">
         <v>145</v>
@@ -7362,7 +7362,7 @@
     <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48925</v>
+        <v>48935</v>
       </c>
       <c r="C153" s="5">
         <v>146</v>
@@ -7395,7 +7395,7 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48956</v>
+        <v>48966</v>
       </c>
       <c r="C154" s="5">
         <v>147</v>
@@ -7428,7 +7428,7 @@
     <row r="155" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B155" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48987</v>
+        <v>48997</v>
       </c>
       <c r="C155" s="5">
         <v>148</v>
@@ -7461,7 +7461,7 @@
     <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49015</v>
+        <v>49025</v>
       </c>
       <c r="C156" s="5">
         <v>149</v>
@@ -7494,7 +7494,7 @@
     <row r="157" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B157" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49046</v>
+        <v>49056</v>
       </c>
       <c r="C157" s="5">
         <v>150</v>
@@ -7527,7 +7527,7 @@
     <row r="158" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B158" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49076</v>
+        <v>49086</v>
       </c>
       <c r="C158" s="5">
         <v>151</v>
@@ -7560,7 +7560,7 @@
     <row r="159" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B159" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49107</v>
+        <v>49117</v>
       </c>
       <c r="C159" s="5">
         <v>152</v>
@@ -7593,7 +7593,7 @@
     <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49137</v>
+        <v>49147</v>
       </c>
       <c r="C160" s="5">
         <v>153</v>
@@ -7626,7 +7626,7 @@
     <row r="161" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B161" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49168</v>
+        <v>49178</v>
       </c>
       <c r="C161" s="5">
         <v>154</v>
@@ -7659,7 +7659,7 @@
     <row r="162" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B162" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49199</v>
+        <v>49209</v>
       </c>
       <c r="C162" s="5">
         <v>155</v>
@@ -7692,7 +7692,7 @@
     <row r="163" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B163" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49229</v>
+        <v>49239</v>
       </c>
       <c r="C163" s="5">
         <v>156</v>
@@ -7725,7 +7725,7 @@
     <row r="164" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B164" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49260</v>
+        <v>49270</v>
       </c>
       <c r="C164" s="5">
         <v>157</v>
@@ -7758,7 +7758,7 @@
     <row r="165" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B165" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49290</v>
+        <v>49300</v>
       </c>
       <c r="C165" s="5">
         <v>158</v>
@@ -7791,7 +7791,7 @@
     <row r="166" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B166" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49321</v>
+        <v>49331</v>
       </c>
       <c r="C166" s="5">
         <v>159</v>
@@ -7824,7 +7824,7 @@
     <row r="167" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B167" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49352</v>
+        <v>49362</v>
       </c>
       <c r="C167" s="5">
         <v>160</v>
@@ -7857,7 +7857,7 @@
     <row r="168" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B168" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49380</v>
+        <v>49390</v>
       </c>
       <c r="C168" s="5">
         <v>161</v>
@@ -7890,7 +7890,7 @@
     <row r="169" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B169" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49411</v>
+        <v>49421</v>
       </c>
       <c r="C169" s="5">
         <v>162</v>
@@ -7923,7 +7923,7 @@
     <row r="170" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B170" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49441</v>
+        <v>49451</v>
       </c>
       <c r="C170" s="5">
         <v>163</v>
@@ -7956,7 +7956,7 @@
     <row r="171" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B171" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49472</v>
+        <v>49482</v>
       </c>
       <c r="C171" s="5">
         <v>164</v>
@@ -7989,7 +7989,7 @@
     <row r="172" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B172" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49502</v>
+        <v>49512</v>
       </c>
       <c r="C172" s="5">
         <v>165</v>
@@ -8022,7 +8022,7 @@
     <row r="173" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B173" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49533</v>
+        <v>49543</v>
       </c>
       <c r="C173" s="5">
         <v>166</v>
@@ -8055,7 +8055,7 @@
     <row r="174" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B174" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49564</v>
+        <v>49574</v>
       </c>
       <c r="C174" s="5">
         <v>167</v>
@@ -8088,7 +8088,7 @@
     <row r="175" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B175" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49594</v>
+        <v>49604</v>
       </c>
       <c r="C175" s="5">
         <v>168</v>
@@ -8121,7 +8121,7 @@
     <row r="176" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B176" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49625</v>
+        <v>49635</v>
       </c>
       <c r="C176" s="5">
         <v>169</v>
@@ -8154,7 +8154,7 @@
     <row r="177" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B177" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49655</v>
+        <v>49665</v>
       </c>
       <c r="C177" s="5">
         <v>170</v>
@@ -8187,7 +8187,7 @@
     <row r="178" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B178" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49686</v>
+        <v>49696</v>
       </c>
       <c r="C178" s="5">
         <v>171</v>
@@ -8220,7 +8220,7 @@
     <row r="179" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B179" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49717</v>
+        <v>49727</v>
       </c>
       <c r="C179" s="5">
         <v>172</v>
@@ -8253,7 +8253,7 @@
     <row r="180" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B180" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49746</v>
+        <v>49756</v>
       </c>
       <c r="C180" s="5">
         <v>173</v>
@@ -8286,7 +8286,7 @@
     <row r="181" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B181" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49777</v>
+        <v>49787</v>
       </c>
       <c r="C181" s="5">
         <v>174</v>
@@ -8319,7 +8319,7 @@
     <row r="182" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B182" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49807</v>
+        <v>49817</v>
       </c>
       <c r="C182" s="5">
         <v>175</v>
@@ -8352,7 +8352,7 @@
     <row r="183" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B183" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49838</v>
+        <v>49848</v>
       </c>
       <c r="C183" s="5">
         <v>176</v>
@@ -8385,7 +8385,7 @@
     <row r="184" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B184" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49868</v>
+        <v>49878</v>
       </c>
       <c r="C184" s="5">
         <v>177</v>
@@ -8418,7 +8418,7 @@
     <row r="185" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B185" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49899</v>
+        <v>49909</v>
       </c>
       <c r="C185" s="5">
         <v>178</v>
@@ -8451,7 +8451,7 @@
     <row r="186" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B186" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49930</v>
+        <v>49940</v>
       </c>
       <c r="C186" s="5">
         <v>179</v>
@@ -8484,7 +8484,7 @@
     <row r="187" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B187" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49960</v>
+        <v>49970</v>
       </c>
       <c r="C187" s="5">
         <v>180</v>
@@ -8517,7 +8517,7 @@
     <row r="188" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B188" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49991</v>
+        <v>50001</v>
       </c>
       <c r="C188" s="5">
         <v>181</v>
@@ -8550,7 +8550,7 @@
     <row r="189" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B189" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50021</v>
+        <v>50031</v>
       </c>
       <c r="C189" s="5">
         <v>182</v>
@@ -8583,7 +8583,7 @@
     <row r="190" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B190" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50052</v>
+        <v>50062</v>
       </c>
       <c r="C190" s="5">
         <v>183</v>
@@ -8616,7 +8616,7 @@
     <row r="191" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B191" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50083</v>
+        <v>50093</v>
       </c>
       <c r="C191" s="5">
         <v>184</v>
@@ -8649,7 +8649,7 @@
     <row r="192" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B192" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50111</v>
+        <v>50121</v>
       </c>
       <c r="C192" s="5">
         <v>185</v>
@@ -8682,7 +8682,7 @@
     <row r="193" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B193" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50142</v>
+        <v>50152</v>
       </c>
       <c r="C193" s="5">
         <v>186</v>
@@ -8715,7 +8715,7 @@
     <row r="194" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B194" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50172</v>
+        <v>50182</v>
       </c>
       <c r="C194" s="5">
         <v>187</v>
@@ -8748,7 +8748,7 @@
     <row r="195" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B195" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50203</v>
+        <v>50213</v>
       </c>
       <c r="C195" s="5">
         <v>188</v>
@@ -8781,7 +8781,7 @@
     <row r="196" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B196" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50233</v>
+        <v>50243</v>
       </c>
       <c r="C196" s="5">
         <v>189</v>
@@ -8814,7 +8814,7 @@
     <row r="197" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B197" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50264</v>
+        <v>50274</v>
       </c>
       <c r="C197" s="5">
         <v>190</v>
@@ -8847,7 +8847,7 @@
     <row r="198" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B198" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50295</v>
+        <v>50305</v>
       </c>
       <c r="C198" s="5">
         <v>191</v>
@@ -8880,7 +8880,7 @@
     <row r="199" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B199" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50325</v>
+        <v>50335</v>
       </c>
       <c r="C199" s="5">
         <v>192</v>
@@ -8913,7 +8913,7 @@
     <row r="200" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B200" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50356</v>
+        <v>50366</v>
       </c>
       <c r="C200" s="5">
         <v>193</v>
@@ -8946,7 +8946,7 @@
     <row r="201" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B201" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50386</v>
+        <v>50396</v>
       </c>
       <c r="C201" s="5">
         <v>194</v>
@@ -8979,7 +8979,7 @@
     <row r="202" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B202" s="25">
         <f t="shared" ref="B202:B265" ca="1" si="28">DATE(YEAR(B201),MONTH(B201)+1,DAY(B201))</f>
-        <v>50417</v>
+        <v>50427</v>
       </c>
       <c r="C202" s="5">
         <v>195</v>
@@ -9012,7 +9012,7 @@
     <row r="203" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B203" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50448</v>
+        <v>50458</v>
       </c>
       <c r="C203" s="5">
         <v>196</v>
@@ -9045,7 +9045,7 @@
     <row r="204" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B204" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50476</v>
+        <v>50486</v>
       </c>
       <c r="C204" s="5">
         <v>197</v>
@@ -9078,7 +9078,7 @@
     <row r="205" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B205" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50507</v>
+        <v>50517</v>
       </c>
       <c r="C205" s="5">
         <v>198</v>
@@ -9111,7 +9111,7 @@
     <row r="206" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B206" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50537</v>
+        <v>50547</v>
       </c>
       <c r="C206" s="5">
         <v>199</v>
@@ -9144,7 +9144,7 @@
     <row r="207" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B207" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50568</v>
+        <v>50578</v>
       </c>
       <c r="C207" s="5">
         <v>200</v>
@@ -9177,7 +9177,7 @@
     <row r="208" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B208" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50598</v>
+        <v>50608</v>
       </c>
       <c r="C208" s="5">
         <v>201</v>
@@ -9210,7 +9210,7 @@
     <row r="209" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B209" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50629</v>
+        <v>50639</v>
       </c>
       <c r="C209" s="5">
         <v>202</v>
@@ -9243,7 +9243,7 @@
     <row r="210" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B210" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50660</v>
+        <v>50670</v>
       </c>
       <c r="C210" s="5">
         <v>203</v>
@@ -9276,7 +9276,7 @@
     <row r="211" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B211" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50690</v>
+        <v>50700</v>
       </c>
       <c r="C211" s="5">
         <v>204</v>
@@ -9309,7 +9309,7 @@
     <row r="212" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B212" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50721</v>
+        <v>50731</v>
       </c>
       <c r="C212" s="5">
         <v>205</v>
@@ -9342,7 +9342,7 @@
     <row r="213" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B213" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50751</v>
+        <v>50761</v>
       </c>
       <c r="C213" s="5">
         <v>206</v>
@@ -9375,7 +9375,7 @@
     <row r="214" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B214" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50782</v>
+        <v>50792</v>
       </c>
       <c r="C214" s="5">
         <v>207</v>
@@ -9408,7 +9408,7 @@
     <row r="215" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B215" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50813</v>
+        <v>50823</v>
       </c>
       <c r="C215" s="5">
         <v>208</v>
@@ -9441,7 +9441,7 @@
     <row r="216" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B216" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50841</v>
+        <v>50851</v>
       </c>
       <c r="C216" s="5">
         <v>209</v>
@@ -9474,7 +9474,7 @@
     <row r="217" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B217" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50872</v>
+        <v>50882</v>
       </c>
       <c r="C217" s="5">
         <v>210</v>
@@ -9507,7 +9507,7 @@
     <row r="218" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B218" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50902</v>
+        <v>50912</v>
       </c>
       <c r="C218" s="5">
         <v>211</v>
@@ -9540,7 +9540,7 @@
     <row r="219" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B219" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50933</v>
+        <v>50943</v>
       </c>
       <c r="C219" s="5">
         <v>212</v>
@@ -9573,7 +9573,7 @@
     <row r="220" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B220" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50963</v>
+        <v>50973</v>
       </c>
       <c r="C220" s="5">
         <v>213</v>
@@ -9606,7 +9606,7 @@
     <row r="221" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B221" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50994</v>
+        <v>51004</v>
       </c>
       <c r="C221" s="5">
         <v>214</v>
@@ -9639,7 +9639,7 @@
     <row r="222" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B222" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51025</v>
+        <v>51035</v>
       </c>
       <c r="C222" s="5">
         <v>215</v>
@@ -9672,7 +9672,7 @@
     <row r="223" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B223" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51055</v>
+        <v>51065</v>
       </c>
       <c r="C223" s="5">
         <v>216</v>
@@ -9705,7 +9705,7 @@
     <row r="224" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B224" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51086</v>
+        <v>51096</v>
       </c>
       <c r="C224" s="5">
         <v>217</v>
@@ -9738,7 +9738,7 @@
     <row r="225" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B225" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51116</v>
+        <v>51126</v>
       </c>
       <c r="C225" s="5">
         <v>218</v>
@@ -9771,7 +9771,7 @@
     <row r="226" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B226" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51147</v>
+        <v>51157</v>
       </c>
       <c r="C226" s="5">
         <v>219</v>
@@ -9804,7 +9804,7 @@
     <row r="227" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B227" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51178</v>
+        <v>51188</v>
       </c>
       <c r="C227" s="5">
         <v>220</v>
@@ -9837,7 +9837,7 @@
     <row r="228" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B228" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51207</v>
+        <v>51217</v>
       </c>
       <c r="C228" s="5">
         <v>221</v>
@@ -9870,7 +9870,7 @@
     <row r="229" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B229" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51238</v>
+        <v>51248</v>
       </c>
       <c r="C229" s="5">
         <v>222</v>
@@ -9903,7 +9903,7 @@
     <row r="230" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B230" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51268</v>
+        <v>51278</v>
       </c>
       <c r="C230" s="5">
         <v>223</v>
@@ -9936,7 +9936,7 @@
     <row r="231" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B231" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51299</v>
+        <v>51309</v>
       </c>
       <c r="C231" s="5">
         <v>224</v>
@@ -9969,7 +9969,7 @@
     <row r="232" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B232" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51329</v>
+        <v>51339</v>
       </c>
       <c r="C232" s="5">
         <v>225</v>
@@ -10002,7 +10002,7 @@
     <row r="233" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B233" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51360</v>
+        <v>51370</v>
       </c>
       <c r="C233" s="5">
         <v>226</v>
@@ -10035,7 +10035,7 @@
     <row r="234" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B234" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51391</v>
+        <v>51401</v>
       </c>
       <c r="C234" s="5">
         <v>227</v>
@@ -10068,7 +10068,7 @@
     <row r="235" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B235" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51421</v>
+        <v>51431</v>
       </c>
       <c r="C235" s="5">
         <v>228</v>
@@ -10101,7 +10101,7 @@
     <row r="236" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B236" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51452</v>
+        <v>51462</v>
       </c>
       <c r="C236" s="5">
         <v>229</v>
@@ -10134,7 +10134,7 @@
     <row r="237" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B237" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51482</v>
+        <v>51492</v>
       </c>
       <c r="C237" s="5">
         <v>230</v>
@@ -10167,7 +10167,7 @@
     <row r="238" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B238" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51513</v>
+        <v>51523</v>
       </c>
       <c r="C238" s="5">
         <v>231</v>
@@ -10200,7 +10200,7 @@
     <row r="239" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B239" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51544</v>
+        <v>51554</v>
       </c>
       <c r="C239" s="5">
         <v>232</v>
@@ -10233,7 +10233,7 @@
     <row r="240" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B240" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51572</v>
+        <v>51582</v>
       </c>
       <c r="C240" s="5">
         <v>233</v>
@@ -10266,7 +10266,7 @@
     <row r="241" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B241" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51603</v>
+        <v>51613</v>
       </c>
       <c r="C241" s="5">
         <v>234</v>
@@ -10299,7 +10299,7 @@
     <row r="242" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B242" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51633</v>
+        <v>51643</v>
       </c>
       <c r="C242" s="5">
         <v>235</v>
@@ -10332,7 +10332,7 @@
     <row r="243" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B243" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51664</v>
+        <v>51674</v>
       </c>
       <c r="C243" s="5">
         <v>236</v>
@@ -10365,7 +10365,7 @@
     <row r="244" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B244" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51694</v>
+        <v>51704</v>
       </c>
       <c r="C244" s="5">
         <v>237</v>
@@ -10398,7 +10398,7 @@
     <row r="245" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B245" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51725</v>
+        <v>51735</v>
       </c>
       <c r="C245" s="5">
         <v>238</v>
@@ -10431,7 +10431,7 @@
     <row r="246" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B246" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51756</v>
+        <v>51766</v>
       </c>
       <c r="C246" s="5">
         <v>239</v>
@@ -10464,7 +10464,7 @@
     <row r="247" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B247" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51786</v>
+        <v>51796</v>
       </c>
       <c r="C247" s="5">
         <v>240</v>
@@ -10497,7 +10497,7 @@
     <row r="248" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B248" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51817</v>
+        <v>51827</v>
       </c>
       <c r="C248" s="5">
         <v>241</v>
@@ -10530,7 +10530,7 @@
     <row r="249" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B249" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51847</v>
+        <v>51857</v>
       </c>
       <c r="C249" s="5">
         <v>242</v>
@@ -10563,7 +10563,7 @@
     <row r="250" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B250" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51878</v>
+        <v>51888</v>
       </c>
       <c r="C250" s="5">
         <v>243</v>
@@ -10596,7 +10596,7 @@
     <row r="251" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B251" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51909</v>
+        <v>51919</v>
       </c>
       <c r="C251" s="5">
         <v>244</v>
@@ -10629,7 +10629,7 @@
     <row r="252" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B252" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51937</v>
+        <v>51947</v>
       </c>
       <c r="C252" s="5">
         <v>245</v>
@@ -10662,7 +10662,7 @@
     <row r="253" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B253" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51968</v>
+        <v>51978</v>
       </c>
       <c r="C253" s="5">
         <v>246</v>
@@ -10695,7 +10695,7 @@
     <row r="254" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B254" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51998</v>
+        <v>52008</v>
       </c>
       <c r="C254" s="5">
         <v>247</v>
@@ -10728,7 +10728,7 @@
     <row r="255" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B255" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52029</v>
+        <v>52039</v>
       </c>
       <c r="C255" s="5">
         <v>248</v>
@@ -10761,7 +10761,7 @@
     <row r="256" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B256" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52059</v>
+        <v>52069</v>
       </c>
       <c r="C256" s="5">
         <v>249</v>
@@ -10794,7 +10794,7 @@
     <row r="257" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B257" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52090</v>
+        <v>52100</v>
       </c>
       <c r="C257" s="5">
         <v>250</v>
@@ -10827,7 +10827,7 @@
     <row r="258" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B258" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52121</v>
+        <v>52131</v>
       </c>
       <c r="C258" s="5">
         <v>251</v>
@@ -10860,7 +10860,7 @@
     <row r="259" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B259" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52151</v>
+        <v>52161</v>
       </c>
       <c r="C259" s="5">
         <v>252</v>
@@ -10893,7 +10893,7 @@
     <row r="260" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B260" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52182</v>
+        <v>52192</v>
       </c>
       <c r="C260" s="5">
         <v>253</v>
@@ -10926,7 +10926,7 @@
     <row r="261" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B261" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52212</v>
+        <v>52222</v>
       </c>
       <c r="C261" s="5">
         <v>254</v>
@@ -10959,7 +10959,7 @@
     <row r="262" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B262" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52243</v>
+        <v>52253</v>
       </c>
       <c r="C262" s="5">
         <v>255</v>
@@ -10992,7 +10992,7 @@
     <row r="263" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B263" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52274</v>
+        <v>52284</v>
       </c>
       <c r="C263" s="5">
         <v>256</v>
@@ -11025,7 +11025,7 @@
     <row r="264" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B264" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52302</v>
+        <v>52312</v>
       </c>
       <c r="C264" s="5">
         <v>257</v>
@@ -11058,7 +11058,7 @@
     <row r="265" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B265" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52333</v>
+        <v>52343</v>
       </c>
       <c r="C265" s="5">
         <v>258</v>
@@ -11091,7 +11091,7 @@
     <row r="266" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B266" s="25">
         <f t="shared" ref="B266:B329" ca="1" si="35">DATE(YEAR(B265),MONTH(B265)+1,DAY(B265))</f>
-        <v>52363</v>
+        <v>52373</v>
       </c>
       <c r="C266" s="5">
         <v>259</v>
@@ -11124,7 +11124,7 @@
     <row r="267" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B267" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52394</v>
+        <v>52404</v>
       </c>
       <c r="C267" s="5">
         <v>260</v>
@@ -11157,7 +11157,7 @@
     <row r="268" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B268" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52424</v>
+        <v>52434</v>
       </c>
       <c r="C268" s="5">
         <v>261</v>
@@ -11190,7 +11190,7 @@
     <row r="269" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B269" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52455</v>
+        <v>52465</v>
       </c>
       <c r="C269" s="5">
         <v>262</v>
@@ -11223,7 +11223,7 @@
     <row r="270" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B270" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52486</v>
+        <v>52496</v>
       </c>
       <c r="C270" s="5">
         <v>263</v>
@@ -11256,7 +11256,7 @@
     <row r="271" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B271" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52516</v>
+        <v>52526</v>
       </c>
       <c r="C271" s="5">
         <v>264</v>
@@ -11289,7 +11289,7 @@
     <row r="272" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B272" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52547</v>
+        <v>52557</v>
       </c>
       <c r="C272" s="5">
         <v>265</v>
@@ -11322,7 +11322,7 @@
     <row r="273" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B273" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52577</v>
+        <v>52587</v>
       </c>
       <c r="C273" s="5">
         <v>266</v>
@@ -11355,7 +11355,7 @@
     <row r="274" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B274" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52608</v>
+        <v>52618</v>
       </c>
       <c r="C274" s="5">
         <v>267</v>
@@ -11388,7 +11388,7 @@
     <row r="275" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B275" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52639</v>
+        <v>52649</v>
       </c>
       <c r="C275" s="5">
         <v>268</v>
@@ -11421,7 +11421,7 @@
     <row r="276" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B276" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52668</v>
+        <v>52678</v>
       </c>
       <c r="C276" s="5">
         <v>269</v>
@@ -11454,7 +11454,7 @@
     <row r="277" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B277" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52699</v>
+        <v>52709</v>
       </c>
       <c r="C277" s="5">
         <v>270</v>
@@ -11487,7 +11487,7 @@
     <row r="278" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B278" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52729</v>
+        <v>52739</v>
       </c>
       <c r="C278" s="5">
         <v>271</v>
@@ -11520,7 +11520,7 @@
     <row r="279" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B279" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52760</v>
+        <v>52770</v>
       </c>
       <c r="C279" s="5">
         <v>272</v>
@@ -11553,7 +11553,7 @@
     <row r="280" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B280" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52790</v>
+        <v>52800</v>
       </c>
       <c r="C280" s="5">
         <v>273</v>
@@ -11586,7 +11586,7 @@
     <row r="281" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B281" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52821</v>
+        <v>52831</v>
       </c>
       <c r="C281" s="5">
         <v>274</v>
@@ -11619,7 +11619,7 @@
     <row r="282" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B282" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52852</v>
+        <v>52862</v>
       </c>
       <c r="C282" s="5">
         <v>275</v>
@@ -11652,7 +11652,7 @@
     <row r="283" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B283" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52882</v>
+        <v>52892</v>
       </c>
       <c r="C283" s="5">
         <v>276</v>
@@ -11685,7 +11685,7 @@
     <row r="284" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B284" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52913</v>
+        <v>52923</v>
       </c>
       <c r="C284" s="5">
         <v>277</v>
@@ -11718,7 +11718,7 @@
     <row r="285" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B285" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52943</v>
+        <v>52953</v>
       </c>
       <c r="C285" s="5">
         <v>278</v>
@@ -11751,7 +11751,7 @@
     <row r="286" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B286" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52974</v>
+        <v>52984</v>
       </c>
       <c r="C286" s="5">
         <v>279</v>
@@ -11784,7 +11784,7 @@
     <row r="287" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B287" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53005</v>
+        <v>53015</v>
       </c>
       <c r="C287" s="5">
         <v>280</v>
@@ -11817,7 +11817,7 @@
     <row r="288" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B288" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53033</v>
+        <v>53043</v>
       </c>
       <c r="C288" s="5">
         <v>281</v>
@@ -11850,7 +11850,7 @@
     <row r="289" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B289" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53064</v>
+        <v>53074</v>
       </c>
       <c r="C289" s="5">
         <v>282</v>
@@ -11883,7 +11883,7 @@
     <row r="290" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B290" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53094</v>
+        <v>53104</v>
       </c>
       <c r="C290" s="5">
         <v>283</v>
@@ -11916,7 +11916,7 @@
     <row r="291" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B291" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53125</v>
+        <v>53135</v>
       </c>
       <c r="C291" s="5">
         <v>284</v>
@@ -11949,7 +11949,7 @@
     <row r="292" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B292" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53155</v>
+        <v>53165</v>
       </c>
       <c r="C292" s="5">
         <v>285</v>
@@ -11982,7 +11982,7 @@
     <row r="293" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B293" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53186</v>
+        <v>53196</v>
       </c>
       <c r="C293" s="5">
         <v>286</v>
@@ -12015,7 +12015,7 @@
     <row r="294" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B294" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53217</v>
+        <v>53227</v>
       </c>
       <c r="C294" s="5">
         <v>287</v>
@@ -12048,7 +12048,7 @@
     <row r="295" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B295" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53247</v>
+        <v>53257</v>
       </c>
       <c r="C295" s="5">
         <v>288</v>
@@ -12081,7 +12081,7 @@
     <row r="296" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B296" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53278</v>
+        <v>53288</v>
       </c>
       <c r="C296" s="5">
         <v>289</v>
@@ -12114,7 +12114,7 @@
     <row r="297" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B297" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53308</v>
+        <v>53318</v>
       </c>
       <c r="C297" s="5">
         <v>290</v>
@@ -12147,7 +12147,7 @@
     <row r="298" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B298" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53339</v>
+        <v>53349</v>
       </c>
       <c r="C298" s="5">
         <v>291</v>
@@ -12180,7 +12180,7 @@
     <row r="299" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B299" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53370</v>
+        <v>53380</v>
       </c>
       <c r="C299" s="5">
         <v>292</v>
@@ -12213,7 +12213,7 @@
     <row r="300" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B300" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53398</v>
+        <v>53408</v>
       </c>
       <c r="C300" s="5">
         <v>293</v>
@@ -12246,7 +12246,7 @@
     <row r="301" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B301" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53429</v>
+        <v>53439</v>
       </c>
       <c r="C301" s="5">
         <v>294</v>
@@ -12279,7 +12279,7 @@
     <row r="302" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B302" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53459</v>
+        <v>53469</v>
       </c>
       <c r="C302" s="5">
         <v>295</v>
@@ -12312,7 +12312,7 @@
     <row r="303" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B303" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53490</v>
+        <v>53500</v>
       </c>
       <c r="C303" s="5">
         <v>296</v>
@@ -12345,7 +12345,7 @@
     <row r="304" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B304" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53520</v>
+        <v>53530</v>
       </c>
       <c r="C304" s="5">
         <v>297</v>
@@ -12378,7 +12378,7 @@
     <row r="305" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B305" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53551</v>
+        <v>53561</v>
       </c>
       <c r="C305" s="5">
         <v>298</v>
@@ -12411,7 +12411,7 @@
     <row r="306" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B306" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53582</v>
+        <v>53592</v>
       </c>
       <c r="C306" s="5">
         <v>299</v>
@@ -12444,7 +12444,7 @@
     <row r="307" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B307" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53612</v>
+        <v>53622</v>
       </c>
       <c r="C307" s="5">
         <v>300</v>
@@ -12477,7 +12477,7 @@
     <row r="308" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B308" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53643</v>
+        <v>53653</v>
       </c>
       <c r="C308" s="5">
         <v>301</v>
@@ -12510,7 +12510,7 @@
     <row r="309" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B309" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53673</v>
+        <v>53683</v>
       </c>
       <c r="C309" s="5">
         <v>302</v>
@@ -12543,7 +12543,7 @@
     <row r="310" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B310" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53704</v>
+        <v>53714</v>
       </c>
       <c r="C310" s="5">
         <v>303</v>
@@ -12576,7 +12576,7 @@
     <row r="311" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B311" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53735</v>
+        <v>53745</v>
       </c>
       <c r="C311" s="5">
         <v>304</v>
@@ -12609,7 +12609,7 @@
     <row r="312" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B312" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53763</v>
+        <v>53773</v>
       </c>
       <c r="C312" s="5">
         <v>305</v>
@@ -12642,7 +12642,7 @@
     <row r="313" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B313" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53794</v>
+        <v>53804</v>
       </c>
       <c r="C313" s="5">
         <v>306</v>
@@ -12675,7 +12675,7 @@
     <row r="314" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B314" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53824</v>
+        <v>53834</v>
       </c>
       <c r="C314" s="5">
         <v>307</v>
@@ -12708,7 +12708,7 @@
     <row r="315" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B315" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53855</v>
+        <v>53865</v>
       </c>
       <c r="C315" s="5">
         <v>308</v>
@@ -12741,7 +12741,7 @@
     <row r="316" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B316" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53885</v>
+        <v>53895</v>
       </c>
       <c r="C316" s="5">
         <v>309</v>
@@ -12774,7 +12774,7 @@
     <row r="317" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B317" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53916</v>
+        <v>53926</v>
       </c>
       <c r="C317" s="5">
         <v>310</v>
@@ -12807,7 +12807,7 @@
     <row r="318" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B318" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53947</v>
+        <v>53957</v>
       </c>
       <c r="C318" s="5">
         <v>311</v>
@@ -12840,7 +12840,7 @@
     <row r="319" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B319" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53977</v>
+        <v>53987</v>
       </c>
       <c r="C319" s="5">
         <v>312</v>
@@ -12873,7 +12873,7 @@
     <row r="320" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B320" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54008</v>
+        <v>54018</v>
       </c>
       <c r="C320" s="5">
         <v>313</v>
@@ -12906,7 +12906,7 @@
     <row r="321" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B321" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54038</v>
+        <v>54048</v>
       </c>
       <c r="C321" s="5">
         <v>314</v>
@@ -12939,7 +12939,7 @@
     <row r="322" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B322" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54069</v>
+        <v>54079</v>
       </c>
       <c r="C322" s="5">
         <v>315</v>
@@ -12972,7 +12972,7 @@
     <row r="323" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B323" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54100</v>
+        <v>54110</v>
       </c>
       <c r="C323" s="5">
         <v>316</v>
@@ -13005,7 +13005,7 @@
     <row r="324" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B324" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54129</v>
+        <v>54139</v>
       </c>
       <c r="C324" s="5">
         <v>317</v>
@@ -13038,7 +13038,7 @@
     <row r="325" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B325" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54160</v>
+        <v>54170</v>
       </c>
       <c r="C325" s="5">
         <v>318</v>
@@ -13071,7 +13071,7 @@
     <row r="326" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B326" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54190</v>
+        <v>54200</v>
       </c>
       <c r="C326" s="5">
         <v>319</v>
@@ -13104,7 +13104,7 @@
     <row r="327" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B327" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54221</v>
+        <v>54231</v>
       </c>
       <c r="C327" s="5">
         <v>320</v>
@@ -13137,7 +13137,7 @@
     <row r="328" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B328" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54251</v>
+        <v>54261</v>
       </c>
       <c r="C328" s="5">
         <v>321</v>
@@ -13170,7 +13170,7 @@
     <row r="329" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B329" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54282</v>
+        <v>54292</v>
       </c>
       <c r="C329" s="5">
         <v>322</v>
@@ -13203,7 +13203,7 @@
     <row r="330" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B330" s="25">
         <f t="shared" ref="B330:B367" ca="1" si="42">DATE(YEAR(B329),MONTH(B329)+1,DAY(B329))</f>
-        <v>54313</v>
+        <v>54323</v>
       </c>
       <c r="C330" s="5">
         <v>323</v>
@@ -13236,7 +13236,7 @@
     <row r="331" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B331" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54343</v>
+        <v>54353</v>
       </c>
       <c r="C331" s="5">
         <v>324</v>
@@ -13269,7 +13269,7 @@
     <row r="332" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B332" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54374</v>
+        <v>54384</v>
       </c>
       <c r="C332" s="5">
         <v>325</v>
@@ -13302,7 +13302,7 @@
     <row r="333" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B333" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54404</v>
+        <v>54414</v>
       </c>
       <c r="C333" s="5">
         <v>326</v>
@@ -13335,7 +13335,7 @@
     <row r="334" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B334" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54435</v>
+        <v>54445</v>
       </c>
       <c r="C334" s="5">
         <v>327</v>
@@ -13368,7 +13368,7 @@
     <row r="335" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B335" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54466</v>
+        <v>54476</v>
       </c>
       <c r="C335" s="5">
         <v>328</v>
@@ -13401,7 +13401,7 @@
     <row r="336" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B336" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54494</v>
+        <v>54504</v>
       </c>
       <c r="C336" s="5">
         <v>329</v>
@@ -13434,7 +13434,7 @@
     <row r="337" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B337" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54525</v>
+        <v>54535</v>
       </c>
       <c r="C337" s="5">
         <v>330</v>
@@ -13467,7 +13467,7 @@
     <row r="338" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B338" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54555</v>
+        <v>54565</v>
       </c>
       <c r="C338" s="5">
         <v>331</v>
@@ -13500,7 +13500,7 @@
     <row r="339" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B339" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54586</v>
+        <v>54596</v>
       </c>
       <c r="C339" s="5">
         <v>332</v>
@@ -13533,7 +13533,7 @@
     <row r="340" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B340" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54616</v>
+        <v>54626</v>
       </c>
       <c r="C340" s="5">
         <v>333</v>
@@ -13566,7 +13566,7 @@
     <row r="341" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B341" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54647</v>
+        <v>54657</v>
       </c>
       <c r="C341" s="5">
         <v>334</v>
@@ -13599,7 +13599,7 @@
     <row r="342" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B342" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54678</v>
+        <v>54688</v>
       </c>
       <c r="C342" s="5">
         <v>335</v>
@@ -13632,7 +13632,7 @@
     <row r="343" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B343" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54708</v>
+        <v>54718</v>
       </c>
       <c r="C343" s="5">
         <v>336</v>
@@ -13665,7 +13665,7 @@
     <row r="344" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B344" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54739</v>
+        <v>54749</v>
       </c>
       <c r="C344" s="5">
         <v>337</v>
@@ -13698,7 +13698,7 @@
     <row r="345" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B345" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54769</v>
+        <v>54779</v>
       </c>
       <c r="C345" s="5">
         <v>338</v>
@@ -13731,7 +13731,7 @@
     <row r="346" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B346" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54800</v>
+        <v>54810</v>
       </c>
       <c r="C346" s="5">
         <v>339</v>
@@ -13764,7 +13764,7 @@
     <row r="347" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B347" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54831</v>
+        <v>54841</v>
       </c>
       <c r="C347" s="5">
         <v>340</v>
@@ -13797,7 +13797,7 @@
     <row r="348" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B348" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54859</v>
+        <v>54869</v>
       </c>
       <c r="C348" s="5">
         <v>341</v>
@@ -13830,7 +13830,7 @@
     <row r="349" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B349" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54890</v>
+        <v>54900</v>
       </c>
       <c r="C349" s="5">
         <v>342</v>
@@ -13863,7 +13863,7 @@
     <row r="350" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B350" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54920</v>
+        <v>54930</v>
       </c>
       <c r="C350" s="5">
         <v>343</v>
@@ -13896,7 +13896,7 @@
     <row r="351" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B351" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54951</v>
+        <v>54961</v>
       </c>
       <c r="C351" s="5">
         <v>344</v>
@@ -13929,7 +13929,7 @@
     <row r="352" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B352" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54981</v>
+        <v>54991</v>
       </c>
       <c r="C352" s="5">
         <v>345</v>
@@ -13962,7 +13962,7 @@
     <row r="353" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B353" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55012</v>
+        <v>55022</v>
       </c>
       <c r="C353" s="5">
         <v>346</v>
@@ -13995,7 +13995,7 @@
     <row r="354" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B354" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55043</v>
+        <v>55053</v>
       </c>
       <c r="C354" s="5">
         <v>347</v>
@@ -14028,7 +14028,7 @@
     <row r="355" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B355" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55073</v>
+        <v>55083</v>
       </c>
       <c r="C355" s="5">
         <v>348</v>
@@ -14061,7 +14061,7 @@
     <row r="356" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B356" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55104</v>
+        <v>55114</v>
       </c>
       <c r="C356" s="5">
         <v>349</v>
@@ -14094,7 +14094,7 @@
     <row r="357" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B357" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55134</v>
+        <v>55144</v>
       </c>
       <c r="C357" s="5">
         <v>350</v>
@@ -14127,7 +14127,7 @@
     <row r="358" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B358" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55165</v>
+        <v>55175</v>
       </c>
       <c r="C358" s="5">
         <v>351</v>
@@ -14160,7 +14160,7 @@
     <row r="359" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B359" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55196</v>
+        <v>55206</v>
       </c>
       <c r="C359" s="5">
         <v>352</v>
@@ -14193,7 +14193,7 @@
     <row r="360" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B360" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55224</v>
+        <v>55234</v>
       </c>
       <c r="C360" s="5">
         <v>353</v>
@@ -14226,7 +14226,7 @@
     <row r="361" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B361" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55255</v>
+        <v>55265</v>
       </c>
       <c r="C361" s="5">
         <v>354</v>
@@ -14259,7 +14259,7 @@
     <row r="362" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B362" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55285</v>
+        <v>55295</v>
       </c>
       <c r="C362" s="5">
         <v>355</v>
@@ -14292,7 +14292,7 @@
     <row r="363" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B363" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55316</v>
+        <v>55326</v>
       </c>
       <c r="C363" s="5">
         <v>356</v>
@@ -14325,7 +14325,7 @@
     <row r="364" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B364" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55346</v>
+        <v>55356</v>
       </c>
       <c r="C364" s="5">
         <v>357</v>
@@ -14358,7 +14358,7 @@
     <row r="365" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B365" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55377</v>
+        <v>55387</v>
       </c>
       <c r="C365" s="5">
         <v>358</v>
@@ -14391,7 +14391,7 @@
     <row r="366" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B366" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55408</v>
+        <v>55418</v>
       </c>
       <c r="C366" s="5">
         <v>359</v>
@@ -14424,7 +14424,7 @@
     <row r="367" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B367" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55438</v>
+        <v>55448</v>
       </c>
       <c r="C367" s="5">
         <v>360</v>

</xml_diff>

<commit_message>
OOP files and more organisation
</commit_message>
<xml_diff>
--- a/Finance-TP1-RAROC.xlsx
+++ b/Finance-TP1-RAROC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentin/Desktop/TSP/3A/Risques financiers/tp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00B118A-1276-214E-9E93-335482BC042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607CFC1A-8B7F-E64F-94AF-EFBA2378FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="26660" windowHeight="16900" xr2:uid="{06508FD0-9F33-7140-9185-849472C81A33}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="26660" windowHeight="16900" activeTab="1" xr2:uid="{06508FD0-9F33-7140-9185-849472C81A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1725,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C23A7D-3D07-8A41-8AFD-1D20132EF969}">
   <dimension ref="A2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1900,7 +1900,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="14">
-        <v>5.8625526106749093E-2</v>
+        <v>5.86255261067491E-2</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>10</v>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="C10">
         <f>Price*montant</f>
-        <v>58625.526106749094</v>
+        <v>58625.526106749101</v>
       </c>
       <c r="H10" s="20" t="s">
         <v>12</v>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C31" s="12">
         <f>(PNB-Couts-EL)/UL+TSR</f>
-        <v>1.033066378330094E-2</v>
+        <v>1.033066378330097E-2</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>55</v>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="C45" s="12">
         <f>(PNB_SB-CoST_SB+PNB-Couts-EL)/UL+TSR</f>
-        <v>0.12000099999999994</v>
+        <v>0.12000100000000007</v>
       </c>
     </row>
   </sheetData>
@@ -2453,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5C48E9-D627-B141-BA85-FA3CA5A8105F}">
   <dimension ref="B2:L367"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,7 +2549,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="25">
         <f ca="1">TODAY()</f>
-        <v>44491</v>
+        <v>44502</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -2577,7 +2577,7 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="25">
         <f ca="1">DATE(YEAR(B7),MONTH(B7)+1,DAY(B7))</f>
-        <v>44522</v>
+        <v>44532</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -2610,7 +2610,7 @@
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="25">
         <f ca="1">DATE(YEAR(B8),MONTH(B8)+1,DAY(B8))</f>
-        <v>44552</v>
+        <v>44563</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
@@ -2643,7 +2643,7 @@
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="25">
         <f t="shared" ref="B10:B73" ca="1" si="6">DATE(YEAR(B9),MONTH(B9)+1,DAY(B9))</f>
-        <v>44583</v>
+        <v>44594</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -2676,7 +2676,7 @@
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
@@ -2709,7 +2709,7 @@
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44642</v>
+        <v>44653</v>
       </c>
       <c r="C12" s="5">
         <v>5</v>
@@ -2742,7 +2742,7 @@
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44673</v>
+        <v>44683</v>
       </c>
       <c r="C13" s="5">
         <v>6</v>
@@ -2775,7 +2775,7 @@
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44703</v>
+        <v>44714</v>
       </c>
       <c r="C14" s="5">
         <v>7</v>
@@ -2808,7 +2808,7 @@
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44734</v>
+        <v>44744</v>
       </c>
       <c r="C15" s="5">
         <v>8</v>
@@ -2841,7 +2841,7 @@
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44764</v>
+        <v>44775</v>
       </c>
       <c r="C16" s="5">
         <v>9</v>
@@ -2874,7 +2874,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44795</v>
+        <v>44806</v>
       </c>
       <c r="C17" s="5">
         <v>10</v>
@@ -2907,7 +2907,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44826</v>
+        <v>44836</v>
       </c>
       <c r="C18" s="5">
         <v>11</v>
@@ -2940,7 +2940,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44856</v>
+        <v>44867</v>
       </c>
       <c r="C19" s="5">
         <v>12</v>
@@ -2973,7 +2973,7 @@
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44887</v>
+        <v>44897</v>
       </c>
       <c r="C20" s="5">
         <v>13</v>
@@ -3006,7 +3006,7 @@
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44917</v>
+        <v>44928</v>
       </c>
       <c r="C21" s="5">
         <v>14</v>
@@ -3039,7 +3039,7 @@
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44948</v>
+        <v>44959</v>
       </c>
       <c r="C22" s="5">
         <v>15</v>
@@ -3072,7 +3072,7 @@
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>44979</v>
+        <v>44987</v>
       </c>
       <c r="C23" s="5">
         <v>16</v>
@@ -3105,7 +3105,7 @@
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45007</v>
+        <v>45018</v>
       </c>
       <c r="C24" s="5">
         <v>17</v>
@@ -3138,7 +3138,7 @@
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45038</v>
+        <v>45048</v>
       </c>
       <c r="C25" s="5">
         <v>18</v>
@@ -3171,7 +3171,7 @@
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45068</v>
+        <v>45079</v>
       </c>
       <c r="C26" s="5">
         <v>19</v>
@@ -3204,7 +3204,7 @@
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45099</v>
+        <v>45109</v>
       </c>
       <c r="C27" s="5">
         <v>20</v>
@@ -3237,7 +3237,7 @@
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45129</v>
+        <v>45140</v>
       </c>
       <c r="C28" s="5">
         <v>21</v>
@@ -3270,7 +3270,7 @@
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45160</v>
+        <v>45171</v>
       </c>
       <c r="C29" s="5">
         <v>22</v>
@@ -3303,7 +3303,7 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45191</v>
+        <v>45201</v>
       </c>
       <c r="C30" s="5">
         <v>23</v>
@@ -3336,7 +3336,7 @@
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45221</v>
+        <v>45232</v>
       </c>
       <c r="C31" s="5">
         <v>24</v>
@@ -3369,7 +3369,7 @@
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45252</v>
+        <v>45262</v>
       </c>
       <c r="C32" s="5">
         <v>25</v>
@@ -3402,7 +3402,7 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45282</v>
+        <v>45293</v>
       </c>
       <c r="C33" s="5">
         <v>26</v>
@@ -3435,7 +3435,7 @@
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45313</v>
+        <v>45324</v>
       </c>
       <c r="C34" s="5">
         <v>27</v>
@@ -3468,7 +3468,7 @@
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45344</v>
+        <v>45353</v>
       </c>
       <c r="C35" s="5">
         <v>28</v>
@@ -3501,7 +3501,7 @@
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45373</v>
+        <v>45384</v>
       </c>
       <c r="C36" s="5">
         <v>29</v>
@@ -3534,7 +3534,7 @@
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45404</v>
+        <v>45414</v>
       </c>
       <c r="C37" s="5">
         <v>30</v>
@@ -3567,7 +3567,7 @@
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="C38" s="5">
         <v>31</v>
@@ -3600,7 +3600,7 @@
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45465</v>
+        <v>45475</v>
       </c>
       <c r="C39" s="5">
         <v>32</v>
@@ -3633,7 +3633,7 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45495</v>
+        <v>45506</v>
       </c>
       <c r="C40" s="5">
         <v>33</v>
@@ -3666,7 +3666,7 @@
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45526</v>
+        <v>45537</v>
       </c>
       <c r="C41" s="5">
         <v>34</v>
@@ -3699,7 +3699,7 @@
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45557</v>
+        <v>45567</v>
       </c>
       <c r="C42" s="5">
         <v>35</v>
@@ -3732,7 +3732,7 @@
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45587</v>
+        <v>45598</v>
       </c>
       <c r="C43" s="5">
         <v>36</v>
@@ -3765,7 +3765,7 @@
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45618</v>
+        <v>45628</v>
       </c>
       <c r="C44" s="5">
         <v>37</v>
@@ -3798,7 +3798,7 @@
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45648</v>
+        <v>45659</v>
       </c>
       <c r="C45" s="5">
         <v>38</v>
@@ -3831,7 +3831,7 @@
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45679</v>
+        <v>45690</v>
       </c>
       <c r="C46" s="5">
         <v>39</v>
@@ -3864,7 +3864,7 @@
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45710</v>
+        <v>45718</v>
       </c>
       <c r="C47" s="5">
         <v>40</v>
@@ -3897,7 +3897,7 @@
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45738</v>
+        <v>45749</v>
       </c>
       <c r="C48" s="5">
         <v>41</v>
@@ -3930,7 +3930,7 @@
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45769</v>
+        <v>45779</v>
       </c>
       <c r="C49" s="5">
         <v>42</v>
@@ -3963,7 +3963,7 @@
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45799</v>
+        <v>45810</v>
       </c>
       <c r="C50" s="5">
         <v>43</v>
@@ -3996,7 +3996,7 @@
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45830</v>
+        <v>45840</v>
       </c>
       <c r="C51" s="5">
         <v>44</v>
@@ -4029,7 +4029,7 @@
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45860</v>
+        <v>45871</v>
       </c>
       <c r="C52" s="5">
         <v>45</v>
@@ -4062,7 +4062,7 @@
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45891</v>
+        <v>45902</v>
       </c>
       <c r="C53" s="5">
         <v>46</v>
@@ -4095,7 +4095,7 @@
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45922</v>
+        <v>45932</v>
       </c>
       <c r="C54" s="5">
         <v>47</v>
@@ -4128,7 +4128,7 @@
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45952</v>
+        <v>45963</v>
       </c>
       <c r="C55" s="5">
         <v>48</v>
@@ -4161,7 +4161,7 @@
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>45983</v>
+        <v>45993</v>
       </c>
       <c r="C56" s="5">
         <v>49</v>
@@ -4194,7 +4194,7 @@
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46013</v>
+        <v>46024</v>
       </c>
       <c r="C57" s="5">
         <v>50</v>
@@ -4227,7 +4227,7 @@
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46044</v>
+        <v>46055</v>
       </c>
       <c r="C58" s="5">
         <v>51</v>
@@ -4260,7 +4260,7 @@
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46075</v>
+        <v>46083</v>
       </c>
       <c r="C59" s="5">
         <v>52</v>
@@ -4293,7 +4293,7 @@
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46103</v>
+        <v>46114</v>
       </c>
       <c r="C60" s="5">
         <v>53</v>
@@ -4326,7 +4326,7 @@
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46134</v>
+        <v>46144</v>
       </c>
       <c r="C61" s="5">
         <v>54</v>
@@ -4359,7 +4359,7 @@
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46164</v>
+        <v>46175</v>
       </c>
       <c r="C62" s="5">
         <v>55</v>
@@ -4392,7 +4392,7 @@
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46195</v>
+        <v>46205</v>
       </c>
       <c r="C63" s="5">
         <v>56</v>
@@ -4425,7 +4425,7 @@
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46225</v>
+        <v>46236</v>
       </c>
       <c r="C64" s="5">
         <v>57</v>
@@ -4458,7 +4458,7 @@
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46256</v>
+        <v>46267</v>
       </c>
       <c r="C65" s="5">
         <v>58</v>
@@ -4491,7 +4491,7 @@
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46287</v>
+        <v>46297</v>
       </c>
       <c r="C66" s="5">
         <v>59</v>
@@ -4524,7 +4524,7 @@
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46317</v>
+        <v>46328</v>
       </c>
       <c r="C67" s="5">
         <v>60</v>
@@ -4557,7 +4557,7 @@
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46348</v>
+        <v>46358</v>
       </c>
       <c r="C68" s="5">
         <v>61</v>
@@ -4590,7 +4590,7 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46378</v>
+        <v>46389</v>
       </c>
       <c r="C69" s="5">
         <v>62</v>
@@ -4623,7 +4623,7 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46409</v>
+        <v>46420</v>
       </c>
       <c r="C70" s="5">
         <v>63</v>
@@ -4656,7 +4656,7 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46440</v>
+        <v>46448</v>
       </c>
       <c r="C71" s="5">
         <v>64</v>
@@ -4689,7 +4689,7 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46468</v>
+        <v>46479</v>
       </c>
       <c r="C72" s="5">
         <v>65</v>
@@ -4722,7 +4722,7 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>46499</v>
+        <v>46509</v>
       </c>
       <c r="C73" s="5">
         <v>66</v>
@@ -4755,7 +4755,7 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="25">
         <f t="shared" ref="B74:B137" ca="1" si="14">DATE(YEAR(B73),MONTH(B73)+1,DAY(B73))</f>
-        <v>46529</v>
+        <v>46540</v>
       </c>
       <c r="C74" s="5">
         <v>67</v>
@@ -4788,7 +4788,7 @@
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46560</v>
+        <v>46570</v>
       </c>
       <c r="C75" s="5">
         <v>68</v>
@@ -4821,7 +4821,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46590</v>
+        <v>46601</v>
       </c>
       <c r="C76" s="5">
         <v>69</v>
@@ -4854,7 +4854,7 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46621</v>
+        <v>46632</v>
       </c>
       <c r="C77" s="5">
         <v>70</v>
@@ -4887,7 +4887,7 @@
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46652</v>
+        <v>46662</v>
       </c>
       <c r="C78" s="5">
         <v>71</v>
@@ -4920,7 +4920,7 @@
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46682</v>
+        <v>46693</v>
       </c>
       <c r="C79" s="5">
         <v>72</v>
@@ -4953,7 +4953,7 @@
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46713</v>
+        <v>46723</v>
       </c>
       <c r="C80" s="5">
         <v>73</v>
@@ -4986,7 +4986,7 @@
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46743</v>
+        <v>46754</v>
       </c>
       <c r="C81" s="5">
         <v>74</v>
@@ -5019,7 +5019,7 @@
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46774</v>
+        <v>46785</v>
       </c>
       <c r="C82" s="5">
         <v>75</v>
@@ -5052,7 +5052,7 @@
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46805</v>
+        <v>46814</v>
       </c>
       <c r="C83" s="5">
         <v>76</v>
@@ -5085,7 +5085,7 @@
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46834</v>
+        <v>46845</v>
       </c>
       <c r="C84" s="5">
         <v>77</v>
@@ -5118,7 +5118,7 @@
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46865</v>
+        <v>46875</v>
       </c>
       <c r="C85" s="5">
         <v>78</v>
@@ -5151,7 +5151,7 @@
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46895</v>
+        <v>46906</v>
       </c>
       <c r="C86" s="5">
         <v>79</v>
@@ -5184,7 +5184,7 @@
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46926</v>
+        <v>46936</v>
       </c>
       <c r="C87" s="5">
         <v>80</v>
@@ -5217,7 +5217,7 @@
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46956</v>
+        <v>46967</v>
       </c>
       <c r="C88" s="5">
         <v>81</v>
@@ -5250,7 +5250,7 @@
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>46987</v>
+        <v>46998</v>
       </c>
       <c r="C89" s="5">
         <v>82</v>
@@ -5283,7 +5283,7 @@
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47018</v>
+        <v>47028</v>
       </c>
       <c r="C90" s="5">
         <v>83</v>
@@ -5316,7 +5316,7 @@
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47048</v>
+        <v>47059</v>
       </c>
       <c r="C91" s="5">
         <v>84</v>
@@ -5349,7 +5349,7 @@
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47079</v>
+        <v>47089</v>
       </c>
       <c r="C92" s="5">
         <v>85</v>
@@ -5382,7 +5382,7 @@
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47109</v>
+        <v>47120</v>
       </c>
       <c r="C93" s="5">
         <v>86</v>
@@ -5415,7 +5415,7 @@
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47140</v>
+        <v>47151</v>
       </c>
       <c r="C94" s="5">
         <v>87</v>
@@ -5448,7 +5448,7 @@
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47171</v>
+        <v>47179</v>
       </c>
       <c r="C95" s="5">
         <v>88</v>
@@ -5481,7 +5481,7 @@
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47199</v>
+        <v>47210</v>
       </c>
       <c r="C96" s="5">
         <v>89</v>
@@ -5514,7 +5514,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47230</v>
+        <v>47240</v>
       </c>
       <c r="C97" s="5">
         <v>90</v>
@@ -5547,7 +5547,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47260</v>
+        <v>47271</v>
       </c>
       <c r="C98" s="5">
         <v>91</v>
@@ -5580,7 +5580,7 @@
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47291</v>
+        <v>47301</v>
       </c>
       <c r="C99" s="5">
         <v>92</v>
@@ -5613,7 +5613,7 @@
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47321</v>
+        <v>47332</v>
       </c>
       <c r="C100" s="5">
         <v>93</v>
@@ -5646,7 +5646,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47352</v>
+        <v>47363</v>
       </c>
       <c r="C101" s="5">
         <v>94</v>
@@ -5679,7 +5679,7 @@
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47383</v>
+        <v>47393</v>
       </c>
       <c r="C102" s="5">
         <v>95</v>
@@ -5712,7 +5712,7 @@
     <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47413</v>
+        <v>47424</v>
       </c>
       <c r="C103" s="5">
         <v>96</v>
@@ -5745,7 +5745,7 @@
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47444</v>
+        <v>47454</v>
       </c>
       <c r="C104" s="5">
         <v>97</v>
@@ -5778,7 +5778,7 @@
     <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47474</v>
+        <v>47485</v>
       </c>
       <c r="C105" s="5">
         <v>98</v>
@@ -5811,7 +5811,7 @@
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47505</v>
+        <v>47516</v>
       </c>
       <c r="C106" s="5">
         <v>99</v>
@@ -5844,7 +5844,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47536</v>
+        <v>47544</v>
       </c>
       <c r="C107" s="5">
         <v>100</v>
@@ -5877,7 +5877,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47564</v>
+        <v>47575</v>
       </c>
       <c r="C108" s="5">
         <v>101</v>
@@ -5910,7 +5910,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47595</v>
+        <v>47605</v>
       </c>
       <c r="C109" s="5">
         <v>102</v>
@@ -5943,7 +5943,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47625</v>
+        <v>47636</v>
       </c>
       <c r="C110" s="5">
         <v>103</v>
@@ -5976,7 +5976,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47656</v>
+        <v>47666</v>
       </c>
       <c r="C111" s="5">
         <v>104</v>
@@ -6009,7 +6009,7 @@
     <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47686</v>
+        <v>47697</v>
       </c>
       <c r="C112" s="5">
         <v>105</v>
@@ -6042,7 +6042,7 @@
     <row r="113" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B113" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47717</v>
+        <v>47728</v>
       </c>
       <c r="C113" s="5">
         <v>106</v>
@@ -6075,7 +6075,7 @@
     <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47748</v>
+        <v>47758</v>
       </c>
       <c r="C114" s="5">
         <v>107</v>
@@ -6108,7 +6108,7 @@
     <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B115" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47778</v>
+        <v>47789</v>
       </c>
       <c r="C115" s="5">
         <v>108</v>
@@ -6141,7 +6141,7 @@
     <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B116" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47809</v>
+        <v>47819</v>
       </c>
       <c r="C116" s="5">
         <v>109</v>
@@ -6174,7 +6174,7 @@
     <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47839</v>
+        <v>47850</v>
       </c>
       <c r="C117" s="5">
         <v>110</v>
@@ -6207,7 +6207,7 @@
     <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B118" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47870</v>
+        <v>47881</v>
       </c>
       <c r="C118" s="5">
         <v>111</v>
@@ -6240,7 +6240,7 @@
     <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47901</v>
+        <v>47909</v>
       </c>
       <c r="C119" s="5">
         <v>112</v>
@@ -6273,7 +6273,7 @@
     <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47929</v>
+        <v>47940</v>
       </c>
       <c r="C120" s="5">
         <v>113</v>
@@ -6306,7 +6306,7 @@
     <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47960</v>
+        <v>47970</v>
       </c>
       <c r="C121" s="5">
         <v>114</v>
@@ -6339,7 +6339,7 @@
     <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>47990</v>
+        <v>48001</v>
       </c>
       <c r="C122" s="5">
         <v>115</v>
@@ -6372,7 +6372,7 @@
     <row r="123" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B123" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48021</v>
+        <v>48031</v>
       </c>
       <c r="C123" s="5">
         <v>116</v>
@@ -6405,7 +6405,7 @@
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48051</v>
+        <v>48062</v>
       </c>
       <c r="C124" s="5">
         <v>117</v>
@@ -6438,7 +6438,7 @@
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48082</v>
+        <v>48093</v>
       </c>
       <c r="C125" s="5">
         <v>118</v>
@@ -6471,7 +6471,7 @@
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48113</v>
+        <v>48123</v>
       </c>
       <c r="C126" s="5">
         <v>119</v>
@@ -6504,7 +6504,7 @@
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48143</v>
+        <v>48154</v>
       </c>
       <c r="C127" s="5">
         <v>120</v>
@@ -6537,7 +6537,7 @@
     <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48174</v>
+        <v>48184</v>
       </c>
       <c r="C128" s="5">
         <v>121</v>
@@ -6570,7 +6570,7 @@
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48204</v>
+        <v>48215</v>
       </c>
       <c r="C129" s="5">
         <v>122</v>
@@ -6603,7 +6603,7 @@
     <row r="130" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B130" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48235</v>
+        <v>48246</v>
       </c>
       <c r="C130" s="5">
         <v>123</v>
@@ -6636,7 +6636,7 @@
     <row r="131" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B131" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48266</v>
+        <v>48275</v>
       </c>
       <c r="C131" s="5">
         <v>124</v>
@@ -6669,7 +6669,7 @@
     <row r="132" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B132" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48295</v>
+        <v>48306</v>
       </c>
       <c r="C132" s="5">
         <v>125</v>
@@ -6702,7 +6702,7 @@
     <row r="133" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B133" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48326</v>
+        <v>48336</v>
       </c>
       <c r="C133" s="5">
         <v>126</v>
@@ -6735,7 +6735,7 @@
     <row r="134" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B134" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48356</v>
+        <v>48367</v>
       </c>
       <c r="C134" s="5">
         <v>127</v>
@@ -6768,7 +6768,7 @@
     <row r="135" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B135" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48387</v>
+        <v>48397</v>
       </c>
       <c r="C135" s="5">
         <v>128</v>
@@ -6801,7 +6801,7 @@
     <row r="136" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B136" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48417</v>
+        <v>48428</v>
       </c>
       <c r="C136" s="5">
         <v>129</v>
@@ -6834,7 +6834,7 @@
     <row r="137" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B137" s="25">
         <f t="shared" ca="1" si="14"/>
-        <v>48448</v>
+        <v>48459</v>
       </c>
       <c r="C137" s="5">
         <v>130</v>
@@ -6867,7 +6867,7 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B138" s="25">
         <f t="shared" ref="B138:B201" ca="1" si="21">DATE(YEAR(B137),MONTH(B137)+1,DAY(B137))</f>
-        <v>48479</v>
+        <v>48489</v>
       </c>
       <c r="C138" s="5">
         <v>131</v>
@@ -6900,7 +6900,7 @@
     <row r="139" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B139" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48509</v>
+        <v>48520</v>
       </c>
       <c r="C139" s="5">
         <v>132</v>
@@ -6933,7 +6933,7 @@
     <row r="140" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B140" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48540</v>
+        <v>48550</v>
       </c>
       <c r="C140" s="5">
         <v>133</v>
@@ -6966,7 +6966,7 @@
     <row r="141" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B141" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48570</v>
+        <v>48581</v>
       </c>
       <c r="C141" s="5">
         <v>134</v>
@@ -6999,7 +6999,7 @@
     <row r="142" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B142" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48601</v>
+        <v>48612</v>
       </c>
       <c r="C142" s="5">
         <v>135</v>
@@ -7032,7 +7032,7 @@
     <row r="143" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B143" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48632</v>
+        <v>48640</v>
       </c>
       <c r="C143" s="5">
         <v>136</v>
@@ -7065,7 +7065,7 @@
     <row r="144" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B144" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48660</v>
+        <v>48671</v>
       </c>
       <c r="C144" s="5">
         <v>137</v>
@@ -7098,7 +7098,7 @@
     <row r="145" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B145" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48691</v>
+        <v>48701</v>
       </c>
       <c r="C145" s="5">
         <v>138</v>
@@ -7131,7 +7131,7 @@
     <row r="146" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B146" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48721</v>
+        <v>48732</v>
       </c>
       <c r="C146" s="5">
         <v>139</v>
@@ -7164,7 +7164,7 @@
     <row r="147" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B147" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48752</v>
+        <v>48762</v>
       </c>
       <c r="C147" s="5">
         <v>140</v>
@@ -7197,7 +7197,7 @@
     <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48782</v>
+        <v>48793</v>
       </c>
       <c r="C148" s="5">
         <v>141</v>
@@ -7230,7 +7230,7 @@
     <row r="149" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B149" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48813</v>
+        <v>48824</v>
       </c>
       <c r="C149" s="5">
         <v>142</v>
@@ -7263,7 +7263,7 @@
     <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48844</v>
+        <v>48854</v>
       </c>
       <c r="C150" s="5">
         <v>143</v>
@@ -7296,7 +7296,7 @@
     <row r="151" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B151" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48874</v>
+        <v>48885</v>
       </c>
       <c r="C151" s="5">
         <v>144</v>
@@ -7329,7 +7329,7 @@
     <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48905</v>
+        <v>48915</v>
       </c>
       <c r="C152" s="5">
         <v>145</v>
@@ -7362,7 +7362,7 @@
     <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48935</v>
+        <v>48946</v>
       </c>
       <c r="C153" s="5">
         <v>146</v>
@@ -7395,7 +7395,7 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48966</v>
+        <v>48977</v>
       </c>
       <c r="C154" s="5">
         <v>147</v>
@@ -7428,7 +7428,7 @@
     <row r="155" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B155" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>48997</v>
+        <v>49005</v>
       </c>
       <c r="C155" s="5">
         <v>148</v>
@@ -7461,7 +7461,7 @@
     <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49025</v>
+        <v>49036</v>
       </c>
       <c r="C156" s="5">
         <v>149</v>
@@ -7494,7 +7494,7 @@
     <row r="157" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B157" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49056</v>
+        <v>49066</v>
       </c>
       <c r="C157" s="5">
         <v>150</v>
@@ -7527,7 +7527,7 @@
     <row r="158" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B158" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49086</v>
+        <v>49097</v>
       </c>
       <c r="C158" s="5">
         <v>151</v>
@@ -7560,7 +7560,7 @@
     <row r="159" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B159" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49117</v>
+        <v>49127</v>
       </c>
       <c r="C159" s="5">
         <v>152</v>
@@ -7593,7 +7593,7 @@
     <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49147</v>
+        <v>49158</v>
       </c>
       <c r="C160" s="5">
         <v>153</v>
@@ -7626,7 +7626,7 @@
     <row r="161" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B161" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49178</v>
+        <v>49189</v>
       </c>
       <c r="C161" s="5">
         <v>154</v>
@@ -7659,7 +7659,7 @@
     <row r="162" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B162" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49209</v>
+        <v>49219</v>
       </c>
       <c r="C162" s="5">
         <v>155</v>
@@ -7692,7 +7692,7 @@
     <row r="163" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B163" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49239</v>
+        <v>49250</v>
       </c>
       <c r="C163" s="5">
         <v>156</v>
@@ -7725,7 +7725,7 @@
     <row r="164" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B164" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49270</v>
+        <v>49280</v>
       </c>
       <c r="C164" s="5">
         <v>157</v>
@@ -7758,7 +7758,7 @@
     <row r="165" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B165" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49300</v>
+        <v>49311</v>
       </c>
       <c r="C165" s="5">
         <v>158</v>
@@ -7791,7 +7791,7 @@
     <row r="166" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B166" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49331</v>
+        <v>49342</v>
       </c>
       <c r="C166" s="5">
         <v>159</v>
@@ -7824,7 +7824,7 @@
     <row r="167" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B167" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49362</v>
+        <v>49370</v>
       </c>
       <c r="C167" s="5">
         <v>160</v>
@@ -7857,7 +7857,7 @@
     <row r="168" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B168" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49390</v>
+        <v>49401</v>
       </c>
       <c r="C168" s="5">
         <v>161</v>
@@ -7890,7 +7890,7 @@
     <row r="169" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B169" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49421</v>
+        <v>49431</v>
       </c>
       <c r="C169" s="5">
         <v>162</v>
@@ -7923,7 +7923,7 @@
     <row r="170" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B170" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49451</v>
+        <v>49462</v>
       </c>
       <c r="C170" s="5">
         <v>163</v>
@@ -7956,7 +7956,7 @@
     <row r="171" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B171" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49482</v>
+        <v>49492</v>
       </c>
       <c r="C171" s="5">
         <v>164</v>
@@ -7989,7 +7989,7 @@
     <row r="172" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B172" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49512</v>
+        <v>49523</v>
       </c>
       <c r="C172" s="5">
         <v>165</v>
@@ -8022,7 +8022,7 @@
     <row r="173" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B173" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49543</v>
+        <v>49554</v>
       </c>
       <c r="C173" s="5">
         <v>166</v>
@@ -8055,7 +8055,7 @@
     <row r="174" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B174" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49574</v>
+        <v>49584</v>
       </c>
       <c r="C174" s="5">
         <v>167</v>
@@ -8088,7 +8088,7 @@
     <row r="175" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B175" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49604</v>
+        <v>49615</v>
       </c>
       <c r="C175" s="5">
         <v>168</v>
@@ -8121,7 +8121,7 @@
     <row r="176" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B176" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49635</v>
+        <v>49645</v>
       </c>
       <c r="C176" s="5">
         <v>169</v>
@@ -8154,7 +8154,7 @@
     <row r="177" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B177" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49665</v>
+        <v>49676</v>
       </c>
       <c r="C177" s="5">
         <v>170</v>
@@ -8187,7 +8187,7 @@
     <row r="178" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B178" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49696</v>
+        <v>49707</v>
       </c>
       <c r="C178" s="5">
         <v>171</v>
@@ -8220,7 +8220,7 @@
     <row r="179" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B179" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49727</v>
+        <v>49736</v>
       </c>
       <c r="C179" s="5">
         <v>172</v>
@@ -8253,7 +8253,7 @@
     <row r="180" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B180" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49756</v>
+        <v>49767</v>
       </c>
       <c r="C180" s="5">
         <v>173</v>
@@ -8286,7 +8286,7 @@
     <row r="181" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B181" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49787</v>
+        <v>49797</v>
       </c>
       <c r="C181" s="5">
         <v>174</v>
@@ -8319,7 +8319,7 @@
     <row r="182" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B182" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49817</v>
+        <v>49828</v>
       </c>
       <c r="C182" s="5">
         <v>175</v>
@@ -8352,7 +8352,7 @@
     <row r="183" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B183" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49848</v>
+        <v>49858</v>
       </c>
       <c r="C183" s="5">
         <v>176</v>
@@ -8385,7 +8385,7 @@
     <row r="184" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B184" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49878</v>
+        <v>49889</v>
       </c>
       <c r="C184" s="5">
         <v>177</v>
@@ -8418,7 +8418,7 @@
     <row r="185" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B185" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49909</v>
+        <v>49920</v>
       </c>
       <c r="C185" s="5">
         <v>178</v>
@@ -8451,7 +8451,7 @@
     <row r="186" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B186" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49940</v>
+        <v>49950</v>
       </c>
       <c r="C186" s="5">
         <v>179</v>
@@ -8484,7 +8484,7 @@
     <row r="187" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B187" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>49970</v>
+        <v>49981</v>
       </c>
       <c r="C187" s="5">
         <v>180</v>
@@ -8517,7 +8517,7 @@
     <row r="188" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B188" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50001</v>
+        <v>50011</v>
       </c>
       <c r="C188" s="5">
         <v>181</v>
@@ -8550,7 +8550,7 @@
     <row r="189" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B189" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50031</v>
+        <v>50042</v>
       </c>
       <c r="C189" s="5">
         <v>182</v>
@@ -8583,7 +8583,7 @@
     <row r="190" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B190" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50062</v>
+        <v>50073</v>
       </c>
       <c r="C190" s="5">
         <v>183</v>
@@ -8616,7 +8616,7 @@
     <row r="191" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B191" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50093</v>
+        <v>50101</v>
       </c>
       <c r="C191" s="5">
         <v>184</v>
@@ -8649,7 +8649,7 @@
     <row r="192" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B192" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50121</v>
+        <v>50132</v>
       </c>
       <c r="C192" s="5">
         <v>185</v>
@@ -8682,7 +8682,7 @@
     <row r="193" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B193" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50152</v>
+        <v>50162</v>
       </c>
       <c r="C193" s="5">
         <v>186</v>
@@ -8715,7 +8715,7 @@
     <row r="194" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B194" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50182</v>
+        <v>50193</v>
       </c>
       <c r="C194" s="5">
         <v>187</v>
@@ -8748,7 +8748,7 @@
     <row r="195" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B195" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50213</v>
+        <v>50223</v>
       </c>
       <c r="C195" s="5">
         <v>188</v>
@@ -8781,7 +8781,7 @@
     <row r="196" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B196" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50243</v>
+        <v>50254</v>
       </c>
       <c r="C196" s="5">
         <v>189</v>
@@ -8814,7 +8814,7 @@
     <row r="197" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B197" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50274</v>
+        <v>50285</v>
       </c>
       <c r="C197" s="5">
         <v>190</v>
@@ -8847,7 +8847,7 @@
     <row r="198" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B198" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50305</v>
+        <v>50315</v>
       </c>
       <c r="C198" s="5">
         <v>191</v>
@@ -8880,7 +8880,7 @@
     <row r="199" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B199" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50335</v>
+        <v>50346</v>
       </c>
       <c r="C199" s="5">
         <v>192</v>
@@ -8913,7 +8913,7 @@
     <row r="200" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B200" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50366</v>
+        <v>50376</v>
       </c>
       <c r="C200" s="5">
         <v>193</v>
@@ -8946,7 +8946,7 @@
     <row r="201" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B201" s="25">
         <f t="shared" ca="1" si="21"/>
-        <v>50396</v>
+        <v>50407</v>
       </c>
       <c r="C201" s="5">
         <v>194</v>
@@ -8979,7 +8979,7 @@
     <row r="202" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B202" s="25">
         <f t="shared" ref="B202:B265" ca="1" si="28">DATE(YEAR(B201),MONTH(B201)+1,DAY(B201))</f>
-        <v>50427</v>
+        <v>50438</v>
       </c>
       <c r="C202" s="5">
         <v>195</v>
@@ -9012,7 +9012,7 @@
     <row r="203" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B203" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50458</v>
+        <v>50466</v>
       </c>
       <c r="C203" s="5">
         <v>196</v>
@@ -9045,7 +9045,7 @@
     <row r="204" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B204" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50486</v>
+        <v>50497</v>
       </c>
       <c r="C204" s="5">
         <v>197</v>
@@ -9078,7 +9078,7 @@
     <row r="205" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B205" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50517</v>
+        <v>50527</v>
       </c>
       <c r="C205" s="5">
         <v>198</v>
@@ -9111,7 +9111,7 @@
     <row r="206" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B206" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50547</v>
+        <v>50558</v>
       </c>
       <c r="C206" s="5">
         <v>199</v>
@@ -9144,7 +9144,7 @@
     <row r="207" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B207" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50578</v>
+        <v>50588</v>
       </c>
       <c r="C207" s="5">
         <v>200</v>
@@ -9177,7 +9177,7 @@
     <row r="208" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B208" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50608</v>
+        <v>50619</v>
       </c>
       <c r="C208" s="5">
         <v>201</v>
@@ -9210,7 +9210,7 @@
     <row r="209" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B209" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50639</v>
+        <v>50650</v>
       </c>
       <c r="C209" s="5">
         <v>202</v>
@@ -9243,7 +9243,7 @@
     <row r="210" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B210" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50670</v>
+        <v>50680</v>
       </c>
       <c r="C210" s="5">
         <v>203</v>
@@ -9276,7 +9276,7 @@
     <row r="211" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B211" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50700</v>
+        <v>50711</v>
       </c>
       <c r="C211" s="5">
         <v>204</v>
@@ -9309,7 +9309,7 @@
     <row r="212" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B212" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50731</v>
+        <v>50741</v>
       </c>
       <c r="C212" s="5">
         <v>205</v>
@@ -9342,7 +9342,7 @@
     <row r="213" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B213" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50761</v>
+        <v>50772</v>
       </c>
       <c r="C213" s="5">
         <v>206</v>
@@ -9375,7 +9375,7 @@
     <row r="214" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B214" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50792</v>
+        <v>50803</v>
       </c>
       <c r="C214" s="5">
         <v>207</v>
@@ -9408,7 +9408,7 @@
     <row r="215" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B215" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50823</v>
+        <v>50831</v>
       </c>
       <c r="C215" s="5">
         <v>208</v>
@@ -9441,7 +9441,7 @@
     <row r="216" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B216" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50851</v>
+        <v>50862</v>
       </c>
       <c r="C216" s="5">
         <v>209</v>
@@ -9474,7 +9474,7 @@
     <row r="217" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B217" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50882</v>
+        <v>50892</v>
       </c>
       <c r="C217" s="5">
         <v>210</v>
@@ -9507,7 +9507,7 @@
     <row r="218" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B218" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50912</v>
+        <v>50923</v>
       </c>
       <c r="C218" s="5">
         <v>211</v>
@@ -9540,7 +9540,7 @@
     <row r="219" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B219" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50943</v>
+        <v>50953</v>
       </c>
       <c r="C219" s="5">
         <v>212</v>
@@ -9573,7 +9573,7 @@
     <row r="220" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B220" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>50973</v>
+        <v>50984</v>
       </c>
       <c r="C220" s="5">
         <v>213</v>
@@ -9606,7 +9606,7 @@
     <row r="221" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B221" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51004</v>
+        <v>51015</v>
       </c>
       <c r="C221" s="5">
         <v>214</v>
@@ -9639,7 +9639,7 @@
     <row r="222" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B222" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51035</v>
+        <v>51045</v>
       </c>
       <c r="C222" s="5">
         <v>215</v>
@@ -9672,7 +9672,7 @@
     <row r="223" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B223" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51065</v>
+        <v>51076</v>
       </c>
       <c r="C223" s="5">
         <v>216</v>
@@ -9705,7 +9705,7 @@
     <row r="224" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B224" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51096</v>
+        <v>51106</v>
       </c>
       <c r="C224" s="5">
         <v>217</v>
@@ -9738,7 +9738,7 @@
     <row r="225" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B225" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51126</v>
+        <v>51137</v>
       </c>
       <c r="C225" s="5">
         <v>218</v>
@@ -9771,7 +9771,7 @@
     <row r="226" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B226" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51157</v>
+        <v>51168</v>
       </c>
       <c r="C226" s="5">
         <v>219</v>
@@ -9804,7 +9804,7 @@
     <row r="227" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B227" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51188</v>
+        <v>51197</v>
       </c>
       <c r="C227" s="5">
         <v>220</v>
@@ -9837,7 +9837,7 @@
     <row r="228" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B228" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51217</v>
+        <v>51228</v>
       </c>
       <c r="C228" s="5">
         <v>221</v>
@@ -9870,7 +9870,7 @@
     <row r="229" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B229" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51248</v>
+        <v>51258</v>
       </c>
       <c r="C229" s="5">
         <v>222</v>
@@ -9903,7 +9903,7 @@
     <row r="230" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B230" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51278</v>
+        <v>51289</v>
       </c>
       <c r="C230" s="5">
         <v>223</v>
@@ -9936,7 +9936,7 @@
     <row r="231" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B231" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51309</v>
+        <v>51319</v>
       </c>
       <c r="C231" s="5">
         <v>224</v>
@@ -9969,7 +9969,7 @@
     <row r="232" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B232" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51339</v>
+        <v>51350</v>
       </c>
       <c r="C232" s="5">
         <v>225</v>
@@ -10002,7 +10002,7 @@
     <row r="233" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B233" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51370</v>
+        <v>51381</v>
       </c>
       <c r="C233" s="5">
         <v>226</v>
@@ -10035,7 +10035,7 @@
     <row r="234" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B234" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51401</v>
+        <v>51411</v>
       </c>
       <c r="C234" s="5">
         <v>227</v>
@@ -10068,7 +10068,7 @@
     <row r="235" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B235" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51431</v>
+        <v>51442</v>
       </c>
       <c r="C235" s="5">
         <v>228</v>
@@ -10101,7 +10101,7 @@
     <row r="236" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B236" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51462</v>
+        <v>51472</v>
       </c>
       <c r="C236" s="5">
         <v>229</v>
@@ -10134,7 +10134,7 @@
     <row r="237" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B237" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51492</v>
+        <v>51503</v>
       </c>
       <c r="C237" s="5">
         <v>230</v>
@@ -10167,7 +10167,7 @@
     <row r="238" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B238" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51523</v>
+        <v>51534</v>
       </c>
       <c r="C238" s="5">
         <v>231</v>
@@ -10200,7 +10200,7 @@
     <row r="239" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B239" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51554</v>
+        <v>51562</v>
       </c>
       <c r="C239" s="5">
         <v>232</v>
@@ -10233,7 +10233,7 @@
     <row r="240" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B240" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51582</v>
+        <v>51593</v>
       </c>
       <c r="C240" s="5">
         <v>233</v>
@@ -10266,7 +10266,7 @@
     <row r="241" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B241" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51613</v>
+        <v>51623</v>
       </c>
       <c r="C241" s="5">
         <v>234</v>
@@ -10299,7 +10299,7 @@
     <row r="242" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B242" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51643</v>
+        <v>51654</v>
       </c>
       <c r="C242" s="5">
         <v>235</v>
@@ -10332,7 +10332,7 @@
     <row r="243" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B243" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51674</v>
+        <v>51684</v>
       </c>
       <c r="C243" s="5">
         <v>236</v>
@@ -10365,7 +10365,7 @@
     <row r="244" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B244" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51704</v>
+        <v>51715</v>
       </c>
       <c r="C244" s="5">
         <v>237</v>
@@ -10398,7 +10398,7 @@
     <row r="245" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B245" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51735</v>
+        <v>51746</v>
       </c>
       <c r="C245" s="5">
         <v>238</v>
@@ -10431,7 +10431,7 @@
     <row r="246" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B246" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51766</v>
+        <v>51776</v>
       </c>
       <c r="C246" s="5">
         <v>239</v>
@@ -10464,7 +10464,7 @@
     <row r="247" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B247" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51796</v>
+        <v>51807</v>
       </c>
       <c r="C247" s="5">
         <v>240</v>
@@ -10497,7 +10497,7 @@
     <row r="248" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B248" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51827</v>
+        <v>51837</v>
       </c>
       <c r="C248" s="5">
         <v>241</v>
@@ -10530,7 +10530,7 @@
     <row r="249" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B249" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51857</v>
+        <v>51868</v>
       </c>
       <c r="C249" s="5">
         <v>242</v>
@@ -10563,7 +10563,7 @@
     <row r="250" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B250" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51888</v>
+        <v>51899</v>
       </c>
       <c r="C250" s="5">
         <v>243</v>
@@ -10596,7 +10596,7 @@
     <row r="251" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B251" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51919</v>
+        <v>51927</v>
       </c>
       <c r="C251" s="5">
         <v>244</v>
@@ -10629,7 +10629,7 @@
     <row r="252" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B252" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51947</v>
+        <v>51958</v>
       </c>
       <c r="C252" s="5">
         <v>245</v>
@@ -10662,7 +10662,7 @@
     <row r="253" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B253" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>51978</v>
+        <v>51988</v>
       </c>
       <c r="C253" s="5">
         <v>246</v>
@@ -10695,7 +10695,7 @@
     <row r="254" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B254" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52008</v>
+        <v>52019</v>
       </c>
       <c r="C254" s="5">
         <v>247</v>
@@ -10728,7 +10728,7 @@
     <row r="255" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B255" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52039</v>
+        <v>52049</v>
       </c>
       <c r="C255" s="5">
         <v>248</v>
@@ -10761,7 +10761,7 @@
     <row r="256" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B256" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52069</v>
+        <v>52080</v>
       </c>
       <c r="C256" s="5">
         <v>249</v>
@@ -10794,7 +10794,7 @@
     <row r="257" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B257" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52100</v>
+        <v>52111</v>
       </c>
       <c r="C257" s="5">
         <v>250</v>
@@ -10827,7 +10827,7 @@
     <row r="258" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B258" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52131</v>
+        <v>52141</v>
       </c>
       <c r="C258" s="5">
         <v>251</v>
@@ -10860,7 +10860,7 @@
     <row r="259" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B259" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52161</v>
+        <v>52172</v>
       </c>
       <c r="C259" s="5">
         <v>252</v>
@@ -10893,7 +10893,7 @@
     <row r="260" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B260" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52192</v>
+        <v>52202</v>
       </c>
       <c r="C260" s="5">
         <v>253</v>
@@ -10926,7 +10926,7 @@
     <row r="261" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B261" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52222</v>
+        <v>52233</v>
       </c>
       <c r="C261" s="5">
         <v>254</v>
@@ -10959,7 +10959,7 @@
     <row r="262" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B262" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52253</v>
+        <v>52264</v>
       </c>
       <c r="C262" s="5">
         <v>255</v>
@@ -10992,7 +10992,7 @@
     <row r="263" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B263" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52284</v>
+        <v>52292</v>
       </c>
       <c r="C263" s="5">
         <v>256</v>
@@ -11025,7 +11025,7 @@
     <row r="264" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B264" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52312</v>
+        <v>52323</v>
       </c>
       <c r="C264" s="5">
         <v>257</v>
@@ -11058,7 +11058,7 @@
     <row r="265" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B265" s="25">
         <f t="shared" ca="1" si="28"/>
-        <v>52343</v>
+        <v>52353</v>
       </c>
       <c r="C265" s="5">
         <v>258</v>
@@ -11091,7 +11091,7 @@
     <row r="266" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B266" s="25">
         <f t="shared" ref="B266:B329" ca="1" si="35">DATE(YEAR(B265),MONTH(B265)+1,DAY(B265))</f>
-        <v>52373</v>
+        <v>52384</v>
       </c>
       <c r="C266" s="5">
         <v>259</v>
@@ -11124,7 +11124,7 @@
     <row r="267" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B267" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52404</v>
+        <v>52414</v>
       </c>
       <c r="C267" s="5">
         <v>260</v>
@@ -11157,7 +11157,7 @@
     <row r="268" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B268" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52434</v>
+        <v>52445</v>
       </c>
       <c r="C268" s="5">
         <v>261</v>
@@ -11190,7 +11190,7 @@
     <row r="269" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B269" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52465</v>
+        <v>52476</v>
       </c>
       <c r="C269" s="5">
         <v>262</v>
@@ -11223,7 +11223,7 @@
     <row r="270" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B270" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52496</v>
+        <v>52506</v>
       </c>
       <c r="C270" s="5">
         <v>263</v>
@@ -11256,7 +11256,7 @@
     <row r="271" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B271" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52526</v>
+        <v>52537</v>
       </c>
       <c r="C271" s="5">
         <v>264</v>
@@ -11289,7 +11289,7 @@
     <row r="272" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B272" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52557</v>
+        <v>52567</v>
       </c>
       <c r="C272" s="5">
         <v>265</v>
@@ -11322,7 +11322,7 @@
     <row r="273" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B273" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52587</v>
+        <v>52598</v>
       </c>
       <c r="C273" s="5">
         <v>266</v>
@@ -11355,7 +11355,7 @@
     <row r="274" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B274" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52618</v>
+        <v>52629</v>
       </c>
       <c r="C274" s="5">
         <v>267</v>
@@ -11388,7 +11388,7 @@
     <row r="275" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B275" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52649</v>
+        <v>52658</v>
       </c>
       <c r="C275" s="5">
         <v>268</v>
@@ -11421,7 +11421,7 @@
     <row r="276" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B276" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52678</v>
+        <v>52689</v>
       </c>
       <c r="C276" s="5">
         <v>269</v>
@@ -11454,7 +11454,7 @@
     <row r="277" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B277" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52709</v>
+        <v>52719</v>
       </c>
       <c r="C277" s="5">
         <v>270</v>
@@ -11487,7 +11487,7 @@
     <row r="278" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B278" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52739</v>
+        <v>52750</v>
       </c>
       <c r="C278" s="5">
         <v>271</v>
@@ -11520,7 +11520,7 @@
     <row r="279" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B279" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52770</v>
+        <v>52780</v>
       </c>
       <c r="C279" s="5">
         <v>272</v>
@@ -11553,7 +11553,7 @@
     <row r="280" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B280" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52800</v>
+        <v>52811</v>
       </c>
       <c r="C280" s="5">
         <v>273</v>
@@ -11586,7 +11586,7 @@
     <row r="281" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B281" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52831</v>
+        <v>52842</v>
       </c>
       <c r="C281" s="5">
         <v>274</v>
@@ -11619,7 +11619,7 @@
     <row r="282" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B282" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52862</v>
+        <v>52872</v>
       </c>
       <c r="C282" s="5">
         <v>275</v>
@@ -11652,7 +11652,7 @@
     <row r="283" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B283" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52892</v>
+        <v>52903</v>
       </c>
       <c r="C283" s="5">
         <v>276</v>
@@ -11685,7 +11685,7 @@
     <row r="284" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B284" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52923</v>
+        <v>52933</v>
       </c>
       <c r="C284" s="5">
         <v>277</v>
@@ -11718,7 +11718,7 @@
     <row r="285" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B285" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52953</v>
+        <v>52964</v>
       </c>
       <c r="C285" s="5">
         <v>278</v>
@@ -11751,7 +11751,7 @@
     <row r="286" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B286" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>52984</v>
+        <v>52995</v>
       </c>
       <c r="C286" s="5">
         <v>279</v>
@@ -11784,7 +11784,7 @@
     <row r="287" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B287" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53015</v>
+        <v>53023</v>
       </c>
       <c r="C287" s="5">
         <v>280</v>
@@ -11817,7 +11817,7 @@
     <row r="288" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B288" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53043</v>
+        <v>53054</v>
       </c>
       <c r="C288" s="5">
         <v>281</v>
@@ -11850,7 +11850,7 @@
     <row r="289" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B289" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53074</v>
+        <v>53084</v>
       </c>
       <c r="C289" s="5">
         <v>282</v>
@@ -11883,7 +11883,7 @@
     <row r="290" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B290" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53104</v>
+        <v>53115</v>
       </c>
       <c r="C290" s="5">
         <v>283</v>
@@ -11916,7 +11916,7 @@
     <row r="291" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B291" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53135</v>
+        <v>53145</v>
       </c>
       <c r="C291" s="5">
         <v>284</v>
@@ -11949,7 +11949,7 @@
     <row r="292" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B292" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53165</v>
+        <v>53176</v>
       </c>
       <c r="C292" s="5">
         <v>285</v>
@@ -11982,7 +11982,7 @@
     <row r="293" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B293" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53196</v>
+        <v>53207</v>
       </c>
       <c r="C293" s="5">
         <v>286</v>
@@ -12015,7 +12015,7 @@
     <row r="294" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B294" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53227</v>
+        <v>53237</v>
       </c>
       <c r="C294" s="5">
         <v>287</v>
@@ -12048,7 +12048,7 @@
     <row r="295" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B295" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53257</v>
+        <v>53268</v>
       </c>
       <c r="C295" s="5">
         <v>288</v>
@@ -12081,7 +12081,7 @@
     <row r="296" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B296" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53288</v>
+        <v>53298</v>
       </c>
       <c r="C296" s="5">
         <v>289</v>
@@ -12114,7 +12114,7 @@
     <row r="297" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B297" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53318</v>
+        <v>53329</v>
       </c>
       <c r="C297" s="5">
         <v>290</v>
@@ -12147,7 +12147,7 @@
     <row r="298" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B298" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53349</v>
+        <v>53360</v>
       </c>
       <c r="C298" s="5">
         <v>291</v>
@@ -12180,7 +12180,7 @@
     <row r="299" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B299" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53380</v>
+        <v>53388</v>
       </c>
       <c r="C299" s="5">
         <v>292</v>
@@ -12213,7 +12213,7 @@
     <row r="300" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B300" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53408</v>
+        <v>53419</v>
       </c>
       <c r="C300" s="5">
         <v>293</v>
@@ -12246,7 +12246,7 @@
     <row r="301" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B301" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53439</v>
+        <v>53449</v>
       </c>
       <c r="C301" s="5">
         <v>294</v>
@@ -12279,7 +12279,7 @@
     <row r="302" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B302" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53469</v>
+        <v>53480</v>
       </c>
       <c r="C302" s="5">
         <v>295</v>
@@ -12312,7 +12312,7 @@
     <row r="303" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B303" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53500</v>
+        <v>53510</v>
       </c>
       <c r="C303" s="5">
         <v>296</v>
@@ -12345,7 +12345,7 @@
     <row r="304" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B304" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53530</v>
+        <v>53541</v>
       </c>
       <c r="C304" s="5">
         <v>297</v>
@@ -12378,7 +12378,7 @@
     <row r="305" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B305" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53561</v>
+        <v>53572</v>
       </c>
       <c r="C305" s="5">
         <v>298</v>
@@ -12411,7 +12411,7 @@
     <row r="306" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B306" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53592</v>
+        <v>53602</v>
       </c>
       <c r="C306" s="5">
         <v>299</v>
@@ -12444,7 +12444,7 @@
     <row r="307" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B307" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53622</v>
+        <v>53633</v>
       </c>
       <c r="C307" s="5">
         <v>300</v>
@@ -12477,7 +12477,7 @@
     <row r="308" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B308" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53653</v>
+        <v>53663</v>
       </c>
       <c r="C308" s="5">
         <v>301</v>
@@ -12510,7 +12510,7 @@
     <row r="309" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B309" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53683</v>
+        <v>53694</v>
       </c>
       <c r="C309" s="5">
         <v>302</v>
@@ -12543,7 +12543,7 @@
     <row r="310" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B310" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53714</v>
+        <v>53725</v>
       </c>
       <c r="C310" s="5">
         <v>303</v>
@@ -12576,7 +12576,7 @@
     <row r="311" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B311" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53745</v>
+        <v>53753</v>
       </c>
       <c r="C311" s="5">
         <v>304</v>
@@ -12609,7 +12609,7 @@
     <row r="312" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B312" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53773</v>
+        <v>53784</v>
       </c>
       <c r="C312" s="5">
         <v>305</v>
@@ -12642,7 +12642,7 @@
     <row r="313" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B313" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53804</v>
+        <v>53814</v>
       </c>
       <c r="C313" s="5">
         <v>306</v>
@@ -12675,7 +12675,7 @@
     <row r="314" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B314" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53834</v>
+        <v>53845</v>
       </c>
       <c r="C314" s="5">
         <v>307</v>
@@ -12708,7 +12708,7 @@
     <row r="315" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B315" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53865</v>
+        <v>53875</v>
       </c>
       <c r="C315" s="5">
         <v>308</v>
@@ -12741,7 +12741,7 @@
     <row r="316" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B316" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53895</v>
+        <v>53906</v>
       </c>
       <c r="C316" s="5">
         <v>309</v>
@@ -12774,7 +12774,7 @@
     <row r="317" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B317" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53926</v>
+        <v>53937</v>
       </c>
       <c r="C317" s="5">
         <v>310</v>
@@ -12807,7 +12807,7 @@
     <row r="318" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B318" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53957</v>
+        <v>53967</v>
       </c>
       <c r="C318" s="5">
         <v>311</v>
@@ -12840,7 +12840,7 @@
     <row r="319" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B319" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>53987</v>
+        <v>53998</v>
       </c>
       <c r="C319" s="5">
         <v>312</v>
@@ -12873,7 +12873,7 @@
     <row r="320" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B320" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54018</v>
+        <v>54028</v>
       </c>
       <c r="C320" s="5">
         <v>313</v>
@@ -12906,7 +12906,7 @@
     <row r="321" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B321" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54048</v>
+        <v>54059</v>
       </c>
       <c r="C321" s="5">
         <v>314</v>
@@ -12939,7 +12939,7 @@
     <row r="322" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B322" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54079</v>
+        <v>54090</v>
       </c>
       <c r="C322" s="5">
         <v>315</v>
@@ -12972,7 +12972,7 @@
     <row r="323" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B323" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54110</v>
+        <v>54119</v>
       </c>
       <c r="C323" s="5">
         <v>316</v>
@@ -13005,7 +13005,7 @@
     <row r="324" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B324" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54139</v>
+        <v>54150</v>
       </c>
       <c r="C324" s="5">
         <v>317</v>
@@ -13038,7 +13038,7 @@
     <row r="325" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B325" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54170</v>
+        <v>54180</v>
       </c>
       <c r="C325" s="5">
         <v>318</v>
@@ -13071,7 +13071,7 @@
     <row r="326" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B326" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54200</v>
+        <v>54211</v>
       </c>
       <c r="C326" s="5">
         <v>319</v>
@@ -13104,7 +13104,7 @@
     <row r="327" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B327" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54231</v>
+        <v>54241</v>
       </c>
       <c r="C327" s="5">
         <v>320</v>
@@ -13137,7 +13137,7 @@
     <row r="328" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B328" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54261</v>
+        <v>54272</v>
       </c>
       <c r="C328" s="5">
         <v>321</v>
@@ -13170,7 +13170,7 @@
     <row r="329" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B329" s="25">
         <f t="shared" ca="1" si="35"/>
-        <v>54292</v>
+        <v>54303</v>
       </c>
       <c r="C329" s="5">
         <v>322</v>
@@ -13203,7 +13203,7 @@
     <row r="330" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B330" s="25">
         <f t="shared" ref="B330:B367" ca="1" si="42">DATE(YEAR(B329),MONTH(B329)+1,DAY(B329))</f>
-        <v>54323</v>
+        <v>54333</v>
       </c>
       <c r="C330" s="5">
         <v>323</v>
@@ -13236,7 +13236,7 @@
     <row r="331" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B331" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54353</v>
+        <v>54364</v>
       </c>
       <c r="C331" s="5">
         <v>324</v>
@@ -13269,7 +13269,7 @@
     <row r="332" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B332" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54384</v>
+        <v>54394</v>
       </c>
       <c r="C332" s="5">
         <v>325</v>
@@ -13302,7 +13302,7 @@
     <row r="333" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B333" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54414</v>
+        <v>54425</v>
       </c>
       <c r="C333" s="5">
         <v>326</v>
@@ -13335,7 +13335,7 @@
     <row r="334" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B334" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54445</v>
+        <v>54456</v>
       </c>
       <c r="C334" s="5">
         <v>327</v>
@@ -13368,7 +13368,7 @@
     <row r="335" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B335" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54476</v>
+        <v>54484</v>
       </c>
       <c r="C335" s="5">
         <v>328</v>
@@ -13401,7 +13401,7 @@
     <row r="336" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B336" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54504</v>
+        <v>54515</v>
       </c>
       <c r="C336" s="5">
         <v>329</v>
@@ -13434,7 +13434,7 @@
     <row r="337" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B337" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54535</v>
+        <v>54545</v>
       </c>
       <c r="C337" s="5">
         <v>330</v>
@@ -13467,7 +13467,7 @@
     <row r="338" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B338" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54565</v>
+        <v>54576</v>
       </c>
       <c r="C338" s="5">
         <v>331</v>
@@ -13500,7 +13500,7 @@
     <row r="339" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B339" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54596</v>
+        <v>54606</v>
       </c>
       <c r="C339" s="5">
         <v>332</v>
@@ -13533,7 +13533,7 @@
     <row r="340" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B340" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54626</v>
+        <v>54637</v>
       </c>
       <c r="C340" s="5">
         <v>333</v>
@@ -13566,7 +13566,7 @@
     <row r="341" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B341" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54657</v>
+        <v>54668</v>
       </c>
       <c r="C341" s="5">
         <v>334</v>
@@ -13599,7 +13599,7 @@
     <row r="342" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B342" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54688</v>
+        <v>54698</v>
       </c>
       <c r="C342" s="5">
         <v>335</v>
@@ -13632,7 +13632,7 @@
     <row r="343" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B343" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54718</v>
+        <v>54729</v>
       </c>
       <c r="C343" s="5">
         <v>336</v>
@@ -13665,7 +13665,7 @@
     <row r="344" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B344" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54749</v>
+        <v>54759</v>
       </c>
       <c r="C344" s="5">
         <v>337</v>
@@ -13698,7 +13698,7 @@
     <row r="345" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B345" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54779</v>
+        <v>54790</v>
       </c>
       <c r="C345" s="5">
         <v>338</v>
@@ -13731,7 +13731,7 @@
     <row r="346" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B346" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54810</v>
+        <v>54821</v>
       </c>
       <c r="C346" s="5">
         <v>339</v>
@@ -13764,7 +13764,7 @@
     <row r="347" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B347" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54841</v>
+        <v>54849</v>
       </c>
       <c r="C347" s="5">
         <v>340</v>
@@ -13797,7 +13797,7 @@
     <row r="348" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B348" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54869</v>
+        <v>54880</v>
       </c>
       <c r="C348" s="5">
         <v>341</v>
@@ -13830,7 +13830,7 @@
     <row r="349" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B349" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54900</v>
+        <v>54910</v>
       </c>
       <c r="C349" s="5">
         <v>342</v>
@@ -13863,7 +13863,7 @@
     <row r="350" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B350" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54930</v>
+        <v>54941</v>
       </c>
       <c r="C350" s="5">
         <v>343</v>
@@ -13896,7 +13896,7 @@
     <row r="351" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B351" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54961</v>
+        <v>54971</v>
       </c>
       <c r="C351" s="5">
         <v>344</v>
@@ -13929,7 +13929,7 @@
     <row r="352" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B352" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>54991</v>
+        <v>55002</v>
       </c>
       <c r="C352" s="5">
         <v>345</v>
@@ -13962,7 +13962,7 @@
     <row r="353" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B353" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55022</v>
+        <v>55033</v>
       </c>
       <c r="C353" s="5">
         <v>346</v>
@@ -13995,7 +13995,7 @@
     <row r="354" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B354" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55053</v>
+        <v>55063</v>
       </c>
       <c r="C354" s="5">
         <v>347</v>
@@ -14028,7 +14028,7 @@
     <row r="355" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B355" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55083</v>
+        <v>55094</v>
       </c>
       <c r="C355" s="5">
         <v>348</v>
@@ -14061,7 +14061,7 @@
     <row r="356" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B356" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55114</v>
+        <v>55124</v>
       </c>
       <c r="C356" s="5">
         <v>349</v>
@@ -14094,7 +14094,7 @@
     <row r="357" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B357" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55144</v>
+        <v>55155</v>
       </c>
       <c r="C357" s="5">
         <v>350</v>
@@ -14127,7 +14127,7 @@
     <row r="358" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B358" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55175</v>
+        <v>55186</v>
       </c>
       <c r="C358" s="5">
         <v>351</v>
@@ -14160,7 +14160,7 @@
     <row r="359" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B359" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55206</v>
+        <v>55214</v>
       </c>
       <c r="C359" s="5">
         <v>352</v>
@@ -14193,7 +14193,7 @@
     <row r="360" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B360" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55234</v>
+        <v>55245</v>
       </c>
       <c r="C360" s="5">
         <v>353</v>
@@ -14226,7 +14226,7 @@
     <row r="361" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B361" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55265</v>
+        <v>55275</v>
       </c>
       <c r="C361" s="5">
         <v>354</v>
@@ -14259,7 +14259,7 @@
     <row r="362" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B362" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55295</v>
+        <v>55306</v>
       </c>
       <c r="C362" s="5">
         <v>355</v>
@@ -14292,7 +14292,7 @@
     <row r="363" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B363" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55326</v>
+        <v>55336</v>
       </c>
       <c r="C363" s="5">
         <v>356</v>
@@ -14325,7 +14325,7 @@
     <row r="364" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B364" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55356</v>
+        <v>55367</v>
       </c>
       <c r="C364" s="5">
         <v>357</v>
@@ -14358,7 +14358,7 @@
     <row r="365" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B365" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55387</v>
+        <v>55398</v>
       </c>
       <c r="C365" s="5">
         <v>358</v>
@@ -14391,7 +14391,7 @@
     <row r="366" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B366" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55418</v>
+        <v>55428</v>
       </c>
       <c r="C366" s="5">
         <v>359</v>
@@ -14424,7 +14424,7 @@
     <row r="367" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B367" s="25">
         <f t="shared" ca="1" si="42"/>
-        <v>55448</v>
+        <v>55459</v>
       </c>
       <c r="C367" s="5">
         <v>360</v>

</xml_diff>